<commit_message>
Clean up project and add dynamic port configuration
- Add comprehensive .gitignore for temporary files and build artifacts
- Remove macOS system files and temporary artifacts
- Add dynamic port configuration system (port_config.json, dynamic_port.py)
- Add smart startup scripts (smart_start.bat, smart_start.ps1)
- Update frontend with API configuration
- Add documentation for dynamic port setup
- Move PDF files to organized uploads directory
- Clean up unused diagnostic and startup files

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/FORMAL_ALL_OU_COMPANIES.xlsx
+++ b/FORMAL_ALL_OU_COMPANIES.xlsx
@@ -1531,11 +1531,7 @@
           <t>Accounting-Input tax claims(Invoice Currency)-Detail</t>
         </is>
       </c>
-      <c r="AY2" s="2" t="inlineStr">
-        <is>
-          <t>Accounting-Input tax claims(Tax currency)-Detail</t>
-        </is>
-      </c>
+      <c r="AY2" s="2" t="n"/>
       <c r="AZ2" s="2" t="inlineStr">
         <is>
           <t>VAT codes</t>
@@ -1820,11 +1816,7 @@
           <t>核算组-可抵扣：可申报税额（发票币种）明细，若存在多行相同发票唯一键数据会自动合并为一张发票的汇总金额</t>
         </is>
       </c>
-      <c r="AY3" s="6" t="inlineStr">
-        <is>
-          <t>核算组-可抵扣：可申报税额（税务币种）明细，若存在多行相同发票唯一键数据会自动合并为一张发票的汇总金额</t>
-        </is>
-      </c>
+      <c r="AY3" s="6" t="n"/>
       <c r="AZ3" s="6" t="inlineStr">
         <is>
           <t>VAT codes</t>
@@ -2028,13 +2020,13 @@
           <t>Level 8/99 Elizabeth Street, SYDNEY NSW 2000, Australia</t>
         </is>
       </c>
-      <c r="Y5" s="4" t="n"/>
+      <c r="Y5" s="4" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
       <c r="Z5" s="4" t="n"/>
-      <c r="AA5" s="4" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
+      <c r="AA5" s="4" t="n"/>
       <c r="AB5" s="4" t="inlineStr">
         <is>
           <t>LEVEL 5 447 COLLINS STREET, MELBOURNE, 3000, AU</t>
@@ -2056,8 +2048,10 @@
       <c r="AL5" s="4" t="n"/>
       <c r="AM5" s="4" t="n"/>
       <c r="AN5" s="4" t="n"/>
-      <c r="AO5" s="4" t="n">
-        <v>0</v>
+      <c r="AO5" s="4" t="inlineStr">
+        <is>
+          <t>10.00 %</t>
+        </is>
       </c>
       <c r="AP5" s="4" t="n">
         <v>233.17</v>
@@ -2074,11 +2068,7 @@
       <c r="AV5" s="4" t="n"/>
       <c r="AW5" s="4" t="n"/>
       <c r="AX5" s="4" t="n"/>
-      <c r="AY5" s="4" t="inlineStr">
-        <is>
-          <t>A002397.135648723.20251003T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY5" s="4" t="n"/>
       <c r="AZ5" s="4" t="n"/>
       <c r="BA5" s="4" t="n"/>
       <c r="BB5" s="4" t="n"/>
@@ -2139,13 +2129,13 @@
           <t>Level 8/99 Elizabeth Street, SYDNEY NSW 2000, Australia</t>
         </is>
       </c>
-      <c r="Y6" s="4" t="n"/>
+      <c r="Y6" s="4" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
       <c r="Z6" s="4" t="n"/>
-      <c r="AA6" s="4" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
+      <c r="AA6" s="4" t="n"/>
       <c r="AB6" s="4" t="inlineStr">
         <is>
           <t>LEVEL 5 447 COLLINS STREET, MELBOURNE, 3000, AU</t>
@@ -2167,8 +2157,10 @@
       <c r="AL6" s="4" t="n"/>
       <c r="AM6" s="4" t="n"/>
       <c r="AN6" s="4" t="n"/>
-      <c r="AO6" s="4" t="n">
-        <v>0</v>
+      <c r="AO6" s="4" t="inlineStr">
+        <is>
+          <t>10.00 %</t>
+        </is>
       </c>
       <c r="AP6" s="4" t="n">
         <v>222.77</v>
@@ -2185,11 +2177,7 @@
       <c r="AV6" s="4" t="n"/>
       <c r="AW6" s="4" t="n"/>
       <c r="AX6" s="4" t="n"/>
-      <c r="AY6" s="4" t="inlineStr">
-        <is>
-          <t>A002397.135805881.20251006T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY6" s="4" t="n"/>
       <c r="AZ6" s="4" t="n"/>
       <c r="BA6" s="4" t="n"/>
       <c r="BB6" s="4" t="n"/>
@@ -2250,13 +2238,13 @@
           <t>Level 8/99 Elizabeth Street, SYDNEY NSW 2000, Australia</t>
         </is>
       </c>
-      <c r="Y7" s="4" t="n"/>
+      <c r="Y7" s="4" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
       <c r="Z7" s="4" t="n"/>
-      <c r="AA7" s="4" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
+      <c r="AA7" s="4" t="n"/>
       <c r="AB7" s="4" t="inlineStr">
         <is>
           <t>LEVEL 5 447 COLLINS STREET, MELBOURNE, 3000, AU</t>
@@ -2278,8 +2266,10 @@
       <c r="AL7" s="4" t="n"/>
       <c r="AM7" s="4" t="n"/>
       <c r="AN7" s="4" t="n"/>
-      <c r="AO7" s="4" t="n">
-        <v>0</v>
+      <c r="AO7" s="4" t="inlineStr">
+        <is>
+          <t>10.00 %</t>
+        </is>
       </c>
       <c r="AP7" s="4" t="n">
         <v>268.53</v>
@@ -2296,11 +2286,7 @@
       <c r="AV7" s="4" t="n"/>
       <c r="AW7" s="4" t="n"/>
       <c r="AX7" s="4" t="n"/>
-      <c r="AY7" s="4" t="inlineStr">
-        <is>
-          <t>A002397.136088774.20251010T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY7" s="4" t="n"/>
       <c r="AZ7" s="4" t="n"/>
       <c r="BA7" s="4" t="n"/>
       <c r="BB7" s="4" t="n"/>
@@ -2361,13 +2347,13 @@
           <t>Level 8/99 Elizabeth Street, SYDNEY NSW 2000, Australia</t>
         </is>
       </c>
-      <c r="Y8" s="4" t="n"/>
+      <c r="Y8" s="4" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
       <c r="Z8" s="4" t="n"/>
-      <c r="AA8" s="4" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
+      <c r="AA8" s="4" t="n"/>
       <c r="AB8" s="4" t="inlineStr">
         <is>
           <t>LEVEL 5 447 COLLINS STREET, MELBOURNE, 3000, AU</t>
@@ -2389,8 +2375,10 @@
       <c r="AL8" s="4" t="n"/>
       <c r="AM8" s="4" t="n"/>
       <c r="AN8" s="4" t="n"/>
-      <c r="AO8" s="4" t="n">
-        <v>0</v>
+      <c r="AO8" s="4" t="inlineStr">
+        <is>
+          <t>10.00 %</t>
+        </is>
       </c>
       <c r="AP8" s="4" t="n">
         <v>243.83</v>
@@ -2407,11 +2395,7 @@
       <c r="AV8" s="4" t="n"/>
       <c r="AW8" s="4" t="n"/>
       <c r="AX8" s="4" t="n"/>
-      <c r="AY8" s="4" t="inlineStr">
-        <is>
-          <t>A002397.136197000.20251012T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY8" s="4" t="n"/>
       <c r="AZ8" s="4" t="n"/>
       <c r="BA8" s="4" t="n"/>
       <c r="BB8" s="4" t="n"/>
@@ -2472,13 +2456,13 @@
           <t>Level 8/99 Elizabeth Street, SYDNEY NSW 2000, Australia</t>
         </is>
       </c>
-      <c r="Y9" s="4" t="n"/>
+      <c r="Y9" s="4" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
       <c r="Z9" s="4" t="n"/>
-      <c r="AA9" s="4" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
+      <c r="AA9" s="4" t="n"/>
       <c r="AB9" s="4" t="inlineStr">
         <is>
           <t>LEVEL 5 447 COLLINS STREET, MELBOURNE, 3000, AU</t>
@@ -2500,8 +2484,10 @@
       <c r="AL9" s="4" t="n"/>
       <c r="AM9" s="4" t="n"/>
       <c r="AN9" s="4" t="n"/>
-      <c r="AO9" s="4" t="n">
-        <v>0</v>
+      <c r="AO9" s="4" t="inlineStr">
+        <is>
+          <t>10.00 %</t>
+        </is>
       </c>
       <c r="AP9" s="4" t="n">
         <v>269.7</v>
@@ -2518,11 +2504,7 @@
       <c r="AV9" s="4" t="n"/>
       <c r="AW9" s="4" t="n"/>
       <c r="AX9" s="4" t="n"/>
-      <c r="AY9" s="4" t="inlineStr">
-        <is>
-          <t>A002397.136315820.20251014T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY9" s="4" t="n"/>
       <c r="AZ9" s="4" t="n"/>
       <c r="BA9" s="4" t="n"/>
       <c r="BB9" s="4" t="n"/>
@@ -2583,13 +2565,13 @@
           <t>Level 8/99 Elizabeth Street, SYDNEY NSW 2000, Australia</t>
         </is>
       </c>
-      <c r="Y10" s="4" t="n"/>
+      <c r="Y10" s="4" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
       <c r="Z10" s="4" t="n"/>
-      <c r="AA10" s="4" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
+      <c r="AA10" s="4" t="n"/>
       <c r="AB10" s="4" t="inlineStr">
         <is>
           <t>LEVEL 5 447 COLLINS STREET, MELBOURNE, 3000, AU</t>
@@ -2611,8 +2593,10 @@
       <c r="AL10" s="4" t="n"/>
       <c r="AM10" s="4" t="n"/>
       <c r="AN10" s="4" t="n"/>
-      <c r="AO10" s="4" t="n">
-        <v>0</v>
+      <c r="AO10" s="4" t="inlineStr">
+        <is>
+          <t>10.00 %</t>
+        </is>
       </c>
       <c r="AP10" s="4" t="n">
         <v>243.22</v>
@@ -2629,11 +2613,7 @@
       <c r="AV10" s="4" t="n"/>
       <c r="AW10" s="4" t="n"/>
       <c r="AX10" s="4" t="n"/>
-      <c r="AY10" s="4" t="inlineStr">
-        <is>
-          <t>A002397.136526696.20251017T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY10" s="4" t="n"/>
       <c r="AZ10" s="4" t="n"/>
       <c r="BA10" s="4" t="n"/>
       <c r="BB10" s="4" t="n"/>
@@ -2694,13 +2674,13 @@
           <t>Level 8/99 Elizabeth Street, SYDNEY NSW 2000, Australia</t>
         </is>
       </c>
-      <c r="Y11" s="4" t="n"/>
+      <c r="Y11" s="4" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
       <c r="Z11" s="4" t="n"/>
-      <c r="AA11" s="4" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
+      <c r="AA11" s="4" t="n"/>
       <c r="AB11" s="4" t="inlineStr">
         <is>
           <t>LEVEL 5 447 COLLINS STREET, MELBOURNE, 3000, AU</t>
@@ -2722,8 +2702,10 @@
       <c r="AL11" s="4" t="n"/>
       <c r="AM11" s="4" t="n"/>
       <c r="AN11" s="4" t="n"/>
-      <c r="AO11" s="4" t="n">
-        <v>0</v>
+      <c r="AO11" s="4" t="inlineStr">
+        <is>
+          <t>10.00 %</t>
+        </is>
       </c>
       <c r="AP11" s="4" t="n">
         <v>243.86</v>
@@ -2740,11 +2722,7 @@
       <c r="AV11" s="4" t="n"/>
       <c r="AW11" s="4" t="n"/>
       <c r="AX11" s="4" t="n"/>
-      <c r="AY11" s="4" t="inlineStr">
-        <is>
-          <t>A002397.136754242.20251021T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY11" s="4" t="n"/>
       <c r="AZ11" s="4" t="n"/>
       <c r="BA11" s="4" t="n"/>
       <c r="BB11" s="4" t="n"/>
@@ -2805,13 +2783,13 @@
           <t>Level 8/99 Elizabeth Street, SYDNEY NSW 2000, Australia</t>
         </is>
       </c>
-      <c r="Y12" s="4" t="n"/>
+      <c r="Y12" s="4" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
       <c r="Z12" s="4" t="n"/>
-      <c r="AA12" s="4" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
+      <c r="AA12" s="4" t="n"/>
       <c r="AB12" s="4" t="inlineStr">
         <is>
           <t>LEVEL 5 447 COLLINS STREET, MELBOURNE, 3000, AU</t>
@@ -2833,8 +2811,10 @@
       <c r="AL12" s="4" t="n"/>
       <c r="AM12" s="4" t="n"/>
       <c r="AN12" s="4" t="n"/>
-      <c r="AO12" s="4" t="n">
-        <v>0</v>
+      <c r="AO12" s="4" t="inlineStr">
+        <is>
+          <t>10.00 %</t>
+        </is>
       </c>
       <c r="AP12" s="4" t="n">
         <v>233.66</v>
@@ -2851,11 +2831,7 @@
       <c r="AV12" s="4" t="n"/>
       <c r="AW12" s="4" t="n"/>
       <c r="AX12" s="4" t="n"/>
-      <c r="AY12" s="4" t="inlineStr">
-        <is>
-          <t>A002397.136965724.20251024T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY12" s="4" t="n"/>
       <c r="AZ12" s="4" t="n"/>
       <c r="BA12" s="4" t="n"/>
       <c r="BB12" s="4" t="n"/>
@@ -2916,13 +2892,13 @@
           <t>Level 8/99 Elizabeth Street, SYDNEY NSW 2000, Australia</t>
         </is>
       </c>
-      <c r="Y13" s="4" t="n"/>
+      <c r="Y13" s="4" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
       <c r="Z13" s="4" t="n"/>
-      <c r="AA13" s="4" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
+      <c r="AA13" s="4" t="n"/>
       <c r="AB13" s="4" t="inlineStr">
         <is>
           <t>LEVEL 5 447 COLLINS STREET, MELBOURNE, 3000, AU</t>
@@ -2944,8 +2920,10 @@
       <c r="AL13" s="4" t="n"/>
       <c r="AM13" s="4" t="n"/>
       <c r="AN13" s="4" t="n"/>
-      <c r="AO13" s="4" t="n">
-        <v>0</v>
+      <c r="AO13" s="4" t="inlineStr">
+        <is>
+          <t>10.00 %</t>
+        </is>
       </c>
       <c r="AP13" s="4" t="n">
         <v>186.87</v>
@@ -2962,11 +2940,7 @@
       <c r="AV13" s="4" t="n"/>
       <c r="AW13" s="4" t="n"/>
       <c r="AX13" s="4" t="n"/>
-      <c r="AY13" s="4" t="inlineStr">
-        <is>
-          <t>A002397.137128653.20251027T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY13" s="4" t="n"/>
       <c r="AZ13" s="4" t="n"/>
       <c r="BA13" s="4" t="n"/>
       <c r="BB13" s="4" t="n"/>
@@ -3027,13 +3001,13 @@
           <t>Level 8/99 Elizabeth Street, SYDNEY NSW 2000, Australia</t>
         </is>
       </c>
-      <c r="Y14" s="4" t="n"/>
+      <c r="Y14" s="4" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
       <c r="Z14" s="4" t="n"/>
-      <c r="AA14" s="4" t="inlineStr">
-        <is>
-          <t>AUD</t>
-        </is>
-      </c>
+      <c r="AA14" s="4" t="n"/>
       <c r="AB14" s="4" t="inlineStr">
         <is>
           <t>LEVEL 5 447 COLLINS STREET, MELBOURNE, 3000, AU</t>
@@ -3055,8 +3029,10 @@
       <c r="AL14" s="4" t="n"/>
       <c r="AM14" s="4" t="n"/>
       <c r="AN14" s="4" t="n"/>
-      <c r="AO14" s="4" t="n">
-        <v>0</v>
+      <c r="AO14" s="4" t="inlineStr">
+        <is>
+          <t>10.00 %</t>
+        </is>
       </c>
       <c r="AP14" s="4" t="n">
         <v>257.09</v>
@@ -3073,11 +3049,7 @@
       <c r="AV14" s="4" t="n"/>
       <c r="AW14" s="4" t="n"/>
       <c r="AX14" s="4" t="n"/>
-      <c r="AY14" s="4" t="inlineStr">
-        <is>
-          <t>A002397.137353863.20251030T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY14" s="4" t="n"/>
       <c r="AZ14" s="4" t="n"/>
       <c r="BA14" s="4" t="n"/>
       <c r="BB14" s="4" t="n"/>
@@ -3138,13 +3110,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y15" s="4" t="n"/>
+      <c r="Y15" s="4" t="inlineStr">
+        <is>
+          <t>PLN</t>
+        </is>
+      </c>
       <c r="Z15" s="4" t="n"/>
-      <c r="AA15" s="4" t="inlineStr">
-        <is>
-          <t>PLN</t>
-        </is>
-      </c>
+      <c r="AA15" s="4" t="n"/>
       <c r="AB15" s="4" t="inlineStr">
         <is>
           <t>12 VICTORIA BUILDING, HADDINGTON ROAD, DUBLIN 4,, DUBLIN, D04XN32</t>
@@ -3166,8 +3138,10 @@
       <c r="AL15" s="4" t="n"/>
       <c r="AM15" s="4" t="n"/>
       <c r="AN15" s="4" t="n"/>
-      <c r="AO15" s="4" t="n">
-        <v>0</v>
+      <c r="AO15" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP15" s="4" t="n">
         <v>0</v>
@@ -3184,11 +3158,7 @@
       <c r="AV15" s="4" t="n"/>
       <c r="AW15" s="4" t="n"/>
       <c r="AX15" s="4" t="n"/>
-      <c r="AY15" s="4" t="inlineStr">
-        <is>
-          <t>K1066436.136151726.20251012T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY15" s="4" t="n"/>
       <c r="AZ15" s="4" t="n"/>
       <c r="BA15" s="4" t="n"/>
       <c r="BB15" s="4" t="n"/>
@@ -3249,13 +3219,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y16" s="4" t="n"/>
+      <c r="Y16" s="4" t="inlineStr">
+        <is>
+          <t>DKK</t>
+        </is>
+      </c>
       <c r="Z16" s="4" t="n"/>
-      <c r="AA16" s="4" t="inlineStr">
-        <is>
-          <t>DKK</t>
-        </is>
-      </c>
+      <c r="AA16" s="4" t="n"/>
       <c r="AB16" s="4" t="inlineStr">
         <is>
           <t>12 VICTORIA BUILDING, HADDINGTON ROAD, DUBLIN 4,, DUBLIN, D04XN32</t>
@@ -3277,8 +3247,10 @@
       <c r="AL16" s="4" t="n"/>
       <c r="AM16" s="4" t="n"/>
       <c r="AN16" s="4" t="n"/>
-      <c r="AO16" s="4" t="n">
-        <v>0</v>
+      <c r="AO16" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP16" s="4" t="n">
         <v>0</v>
@@ -3295,11 +3267,7 @@
       <c r="AV16" s="4" t="n"/>
       <c r="AW16" s="4" t="n"/>
       <c r="AX16" s="4" t="n"/>
-      <c r="AY16" s="4" t="inlineStr">
-        <is>
-          <t>K1066436.136467277.20251017T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY16" s="4" t="n"/>
       <c r="AZ16" s="4" t="n"/>
       <c r="BA16" s="4" t="n"/>
       <c r="BB16" s="4" t="n"/>
@@ -3360,13 +3328,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y17" s="4" t="n"/>
+      <c r="Y17" s="4" t="inlineStr">
+        <is>
+          <t>PLN</t>
+        </is>
+      </c>
       <c r="Z17" s="4" t="n"/>
-      <c r="AA17" s="4" t="inlineStr">
-        <is>
-          <t>PLN</t>
-        </is>
-      </c>
+      <c r="AA17" s="4" t="n"/>
       <c r="AB17" s="4" t="inlineStr">
         <is>
           <t>12 VICTORIA BUILDING, HADDINGTON ROAD, DUBLIN 4,, DUBLIN, D04XN32</t>
@@ -3388,8 +3356,10 @@
       <c r="AL17" s="4" t="n"/>
       <c r="AM17" s="4" t="n"/>
       <c r="AN17" s="4" t="n"/>
-      <c r="AO17" s="4" t="n">
-        <v>0</v>
+      <c r="AO17" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP17" s="4" t="n">
         <v>0</v>
@@ -3406,11 +3376,7 @@
       <c r="AV17" s="4" t="n"/>
       <c r="AW17" s="4" t="n"/>
       <c r="AX17" s="4" t="n"/>
-      <c r="AY17" s="4" t="inlineStr">
-        <is>
-          <t>K1066436.136529659.20251018T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY17" s="4" t="n"/>
       <c r="AZ17" s="4" t="n"/>
       <c r="BA17" s="4" t="n"/>
       <c r="BB17" s="4" t="n"/>
@@ -3471,13 +3437,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y18" s="4" t="n"/>
+      <c r="Y18" s="4" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
       <c r="Z18" s="4" t="n"/>
-      <c r="AA18" s="4" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
+      <c r="AA18" s="4" t="n"/>
       <c r="AB18" s="4" t="inlineStr">
         <is>
           <t>12 VICTORIA BUILDING, HADDINGTON ROAD, DUBLIN 4,, DUBLIN, D04XN32</t>
@@ -3499,8 +3465,10 @@
       <c r="AL18" s="4" t="n"/>
       <c r="AM18" s="4" t="n"/>
       <c r="AN18" s="4" t="n"/>
-      <c r="AO18" s="4" t="n">
-        <v>0</v>
+      <c r="AO18" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP18" s="4" t="n">
         <v>0</v>
@@ -3517,11 +3485,7 @@
       <c r="AV18" s="4" t="n"/>
       <c r="AW18" s="4" t="n"/>
       <c r="AX18" s="4" t="n"/>
-      <c r="AY18" s="4" t="inlineStr">
-        <is>
-          <t>K1066436.136637608.20251020T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY18" s="4" t="n"/>
       <c r="AZ18" s="4" t="n"/>
       <c r="BA18" s="4" t="n"/>
       <c r="BB18" s="4" t="n"/>
@@ -3582,13 +3546,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y19" s="4" t="n"/>
+      <c r="Y19" s="4" t="inlineStr">
+        <is>
+          <t>RON</t>
+        </is>
+      </c>
       <c r="Z19" s="4" t="n"/>
-      <c r="AA19" s="4" t="inlineStr">
-        <is>
-          <t>RON</t>
-        </is>
-      </c>
+      <c r="AA19" s="4" t="n"/>
       <c r="AB19" s="4" t="inlineStr">
         <is>
           <t>12 VICTORIA BUILDING, HADDINGTON ROAD, DUBLIN 4,, DUBLIN, D04XN32</t>
@@ -3610,8 +3574,10 @@
       <c r="AL19" s="4" t="n"/>
       <c r="AM19" s="4" t="n"/>
       <c r="AN19" s="4" t="n"/>
-      <c r="AO19" s="4" t="n">
-        <v>0</v>
+      <c r="AO19" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP19" s="4" t="n">
         <v>0</v>
@@ -3628,11 +3594,7 @@
       <c r="AV19" s="4" t="n"/>
       <c r="AW19" s="4" t="n"/>
       <c r="AX19" s="4" t="n"/>
-      <c r="AY19" s="4" t="inlineStr">
-        <is>
-          <t>K1066436.136686564.20251021T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY19" s="4" t="n"/>
       <c r="AZ19" s="4" t="n"/>
       <c r="BA19" s="4" t="n"/>
       <c r="BB19" s="4" t="n"/>
@@ -3693,13 +3655,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y20" s="4" t="n"/>
+      <c r="Y20" s="4" t="inlineStr">
+        <is>
+          <t>SEK</t>
+        </is>
+      </c>
       <c r="Z20" s="4" t="n"/>
-      <c r="AA20" s="4" t="inlineStr">
-        <is>
-          <t>SEK</t>
-        </is>
-      </c>
+      <c r="AA20" s="4" t="n"/>
       <c r="AB20" s="4" t="inlineStr">
         <is>
           <t>12 VICTORIA BUILDING, HADDINGTON ROAD, DUBLIN 4,, DUBLIN, D04XN32</t>
@@ -3721,8 +3683,10 @@
       <c r="AL20" s="4" t="n"/>
       <c r="AM20" s="4" t="n"/>
       <c r="AN20" s="4" t="n"/>
-      <c r="AO20" s="4" t="n">
-        <v>0</v>
+      <c r="AO20" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP20" s="4" t="n">
         <v>0</v>
@@ -3739,11 +3703,7 @@
       <c r="AV20" s="4" t="n"/>
       <c r="AW20" s="4" t="n"/>
       <c r="AX20" s="4" t="n"/>
-      <c r="AY20" s="4" t="inlineStr">
-        <is>
-          <t>K1066436.136758211.20251022T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY20" s="4" t="n"/>
       <c r="AZ20" s="4" t="n"/>
       <c r="BA20" s="4" t="n"/>
       <c r="BB20" s="4" t="n"/>
@@ -3804,13 +3764,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y21" s="4" t="n"/>
+      <c r="Y21" s="4" t="inlineStr">
+        <is>
+          <t>CHF</t>
+        </is>
+      </c>
       <c r="Z21" s="4" t="n"/>
-      <c r="AA21" s="4" t="inlineStr">
-        <is>
-          <t>CHF</t>
-        </is>
-      </c>
+      <c r="AA21" s="4" t="n"/>
       <c r="AB21" s="4" t="inlineStr">
         <is>
           <t>12 VICTORIA BUILDING, HADDINGTON ROAD, DUBLIN 4,, DUBLIN, D04XN32</t>
@@ -3832,8 +3792,10 @@
       <c r="AL21" s="4" t="n"/>
       <c r="AM21" s="4" t="n"/>
       <c r="AN21" s="4" t="n"/>
-      <c r="AO21" s="4" t="n">
-        <v>0</v>
+      <c r="AO21" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP21" s="4" t="n">
         <v>0</v>
@@ -3850,11 +3812,7 @@
       <c r="AV21" s="4" t="n"/>
       <c r="AW21" s="4" t="n"/>
       <c r="AX21" s="4" t="n"/>
-      <c r="AY21" s="4" t="inlineStr">
-        <is>
-          <t>K1066436.136823171.20251023T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY21" s="4" t="n"/>
       <c r="AZ21" s="4" t="n"/>
       <c r="BA21" s="4" t="n"/>
       <c r="BB21" s="4" t="n"/>
@@ -3915,13 +3873,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y22" s="4" t="n"/>
+      <c r="Y22" s="4" t="inlineStr">
+        <is>
+          <t>CZK</t>
+        </is>
+      </c>
       <c r="Z22" s="4" t="n"/>
-      <c r="AA22" s="4" t="inlineStr">
-        <is>
-          <t>CZK</t>
-        </is>
-      </c>
+      <c r="AA22" s="4" t="n"/>
       <c r="AB22" s="4" t="inlineStr">
         <is>
           <t>12 VICTORIA BUILDING, HADDINGTON ROAD, DUBLIN 4,, DUBLIN, D04XN32</t>
@@ -3943,8 +3901,10 @@
       <c r="AL22" s="4" t="n"/>
       <c r="AM22" s="4" t="n"/>
       <c r="AN22" s="4" t="n"/>
-      <c r="AO22" s="4" t="n">
-        <v>0</v>
+      <c r="AO22" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP22" s="4" t="n">
         <v>0</v>
@@ -3961,11 +3921,7 @@
       <c r="AV22" s="4" t="n"/>
       <c r="AW22" s="4" t="n"/>
       <c r="AX22" s="4" t="n"/>
-      <c r="AY22" s="4" t="inlineStr">
-        <is>
-          <t>K1066436.137031716.20251026T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY22" s="4" t="n"/>
       <c r="AZ22" s="4" t="n"/>
       <c r="BA22" s="4" t="n"/>
       <c r="BB22" s="4" t="n"/>
@@ -4026,13 +3982,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y23" s="4" t="n"/>
+      <c r="Y23" s="4" t="inlineStr">
+        <is>
+          <t>CZK</t>
+        </is>
+      </c>
       <c r="Z23" s="4" t="n"/>
-      <c r="AA23" s="4" t="inlineStr">
-        <is>
-          <t>CZK</t>
-        </is>
-      </c>
+      <c r="AA23" s="4" t="n"/>
       <c r="AB23" s="4" t="inlineStr">
         <is>
           <t>12 VICTORIA BUILDING, HADDINGTON ROAD, DUBLIN 4,, DUBLIN, D04XN32</t>
@@ -4054,8 +4010,10 @@
       <c r="AL23" s="4" t="n"/>
       <c r="AM23" s="4" t="n"/>
       <c r="AN23" s="4" t="n"/>
-      <c r="AO23" s="4" t="n">
-        <v>0</v>
+      <c r="AO23" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP23" s="4" t="n">
         <v>0</v>
@@ -4072,11 +4030,7 @@
       <c r="AV23" s="4" t="n"/>
       <c r="AW23" s="4" t="n"/>
       <c r="AX23" s="4" t="n"/>
-      <c r="AY23" s="4" t="inlineStr">
-        <is>
-          <t>K1066436.137080924.20251027T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY23" s="4" t="n"/>
       <c r="AZ23" s="4" t="n"/>
       <c r="BA23" s="4" t="n"/>
       <c r="BB23" s="4" t="n"/>
@@ -4137,13 +4091,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y24" s="4" t="n"/>
+      <c r="Y24" s="4" t="inlineStr">
+        <is>
+          <t>SEK</t>
+        </is>
+      </c>
       <c r="Z24" s="4" t="n"/>
-      <c r="AA24" s="4" t="inlineStr">
-        <is>
-          <t>SEK</t>
-        </is>
-      </c>
+      <c r="AA24" s="4" t="n"/>
       <c r="AB24" s="4" t="inlineStr">
         <is>
           <t>12 VICTORIA BUILDING, HADDINGTON ROAD, DUBLIN 4,, DUBLIN, D04XN32</t>
@@ -4165,8 +4119,10 @@
       <c r="AL24" s="4" t="n"/>
       <c r="AM24" s="4" t="n"/>
       <c r="AN24" s="4" t="n"/>
-      <c r="AO24" s="4" t="n">
-        <v>0</v>
+      <c r="AO24" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP24" s="4" t="n">
         <v>0</v>
@@ -4183,11 +4139,7 @@
       <c r="AV24" s="4" t="n"/>
       <c r="AW24" s="4" t="n"/>
       <c r="AX24" s="4" t="n"/>
-      <c r="AY24" s="4" t="inlineStr">
-        <is>
-          <t>K1066436.137133936.20251028T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY24" s="4" t="n"/>
       <c r="AZ24" s="4" t="n"/>
       <c r="BA24" s="4" t="n"/>
       <c r="BB24" s="4" t="n"/>
@@ -4248,13 +4200,13 @@
           <t>7th Floor, 33 Cavendish Square, London W1G 0PW, United Kingdom</t>
         </is>
       </c>
-      <c r="Y25" s="4" t="n"/>
+      <c r="Y25" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z25" s="4" t="n"/>
-      <c r="AA25" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA25" s="4" t="n"/>
       <c r="AB25" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -4276,8 +4228,10 @@
       <c r="AL25" s="4" t="n"/>
       <c r="AM25" s="4" t="n"/>
       <c r="AN25" s="4" t="n"/>
-      <c r="AO25" s="4" t="n">
-        <v>0</v>
+      <c r="AO25" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP25" s="4" t="n">
         <v>14467.3</v>
@@ -4294,11 +4248,7 @@
       <c r="AV25" s="4" t="n"/>
       <c r="AW25" s="4" t="n"/>
       <c r="AX25" s="4" t="n"/>
-      <c r="AY25" s="4" t="inlineStr">
-        <is>
-          <t>K1115289.135442254.20251001T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY25" s="4" t="n"/>
       <c r="AZ25" s="4" t="n"/>
       <c r="BA25" s="4" t="n"/>
       <c r="BB25" s="4" t="n"/>
@@ -4359,13 +4309,13 @@
           <t>7th Floor, 33 Cavendish Square, London W1G 0PW, United Kingdom</t>
         </is>
       </c>
-      <c r="Y26" s="4" t="n"/>
+      <c r="Y26" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z26" s="4" t="n"/>
-      <c r="AA26" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA26" s="4" t="n"/>
       <c r="AB26" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -4387,8 +4337,10 @@
       <c r="AL26" s="4" t="n"/>
       <c r="AM26" s="4" t="n"/>
       <c r="AN26" s="4" t="n"/>
-      <c r="AO26" s="4" t="n">
-        <v>0</v>
+      <c r="AO26" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP26" s="4" t="n">
         <v>12278.42</v>
@@ -4405,11 +4357,7 @@
       <c r="AV26" s="4" t="n"/>
       <c r="AW26" s="4" t="n"/>
       <c r="AX26" s="4" t="n"/>
-      <c r="AY26" s="4" t="inlineStr">
-        <is>
-          <t>K1115289.135591436.20251003T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY26" s="4" t="n"/>
       <c r="AZ26" s="4" t="n"/>
       <c r="BA26" s="4" t="n"/>
       <c r="BB26" s="4" t="n"/>
@@ -4470,13 +4418,13 @@
           <t>7th Floor, 33 Cavendish Square, London W1G 0PW, United Kingdom</t>
         </is>
       </c>
-      <c r="Y27" s="4" t="n"/>
+      <c r="Y27" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z27" s="4" t="n"/>
-      <c r="AA27" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA27" s="4" t="n"/>
       <c r="AB27" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -4498,8 +4446,10 @@
       <c r="AL27" s="4" t="n"/>
       <c r="AM27" s="4" t="n"/>
       <c r="AN27" s="4" t="n"/>
-      <c r="AO27" s="4" t="n">
-        <v>0</v>
+      <c r="AO27" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP27" s="4" t="n">
         <v>12533.76</v>
@@ -4516,11 +4466,7 @@
       <c r="AV27" s="4" t="n"/>
       <c r="AW27" s="4" t="n"/>
       <c r="AX27" s="4" t="n"/>
-      <c r="AY27" s="4" t="inlineStr">
-        <is>
-          <t>K1115289.135713223.20251005T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY27" s="4" t="n"/>
       <c r="AZ27" s="4" t="n"/>
       <c r="BA27" s="4" t="n"/>
       <c r="BB27" s="4" t="n"/>
@@ -4581,13 +4527,13 @@
           <t>7th Floor, 33 Cavendish Square, London W1G 0PW, United Kingdom</t>
         </is>
       </c>
-      <c r="Y28" s="4" t="n"/>
+      <c r="Y28" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z28" s="4" t="n"/>
-      <c r="AA28" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA28" s="4" t="n"/>
       <c r="AB28" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -4609,8 +4555,10 @@
       <c r="AL28" s="4" t="n"/>
       <c r="AM28" s="4" t="n"/>
       <c r="AN28" s="4" t="n"/>
-      <c r="AO28" s="4" t="n">
-        <v>0</v>
+      <c r="AO28" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP28" s="4" t="n">
         <v>11439.75</v>
@@ -4627,11 +4575,7 @@
       <c r="AV28" s="4" t="n"/>
       <c r="AW28" s="4" t="n"/>
       <c r="AX28" s="4" t="n"/>
-      <c r="AY28" s="4" t="inlineStr">
-        <is>
-          <t>K1115289.135814724.20251007T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY28" s="4" t="n"/>
       <c r="AZ28" s="4" t="n"/>
       <c r="BA28" s="4" t="n"/>
       <c r="BB28" s="4" t="n"/>
@@ -4692,13 +4636,13 @@
           <t>7th Floor, 33 Cavendish Square, London W1G 0PW, United Kingdom</t>
         </is>
       </c>
-      <c r="Y29" s="4" t="n"/>
+      <c r="Y29" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z29" s="4" t="n"/>
-      <c r="AA29" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA29" s="4" t="n"/>
       <c r="AB29" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -4720,8 +4664,10 @@
       <c r="AL29" s="4" t="n"/>
       <c r="AM29" s="4" t="n"/>
       <c r="AN29" s="4" t="n"/>
-      <c r="AO29" s="4" t="n">
-        <v>0</v>
+      <c r="AO29" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP29" s="4" t="n">
         <v>10712.94</v>
@@ -4738,11 +4684,7 @@
       <c r="AV29" s="4" t="n"/>
       <c r="AW29" s="4" t="n"/>
       <c r="AX29" s="4" t="n"/>
-      <c r="AY29" s="4" t="inlineStr">
-        <is>
-          <t>K1115289.135965110.20251009T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY29" s="4" t="n"/>
       <c r="AZ29" s="4" t="n"/>
       <c r="BA29" s="4" t="n"/>
       <c r="BB29" s="4" t="n"/>
@@ -4803,13 +4745,13 @@
           <t>7th Floor, 33 Cavendish Square, London W1G 0PW, United Kingdom</t>
         </is>
       </c>
-      <c r="Y30" s="4" t="n"/>
+      <c r="Y30" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z30" s="4" t="n"/>
-      <c r="AA30" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA30" s="4" t="n"/>
       <c r="AB30" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -4831,8 +4773,10 @@
       <c r="AL30" s="4" t="n"/>
       <c r="AM30" s="4" t="n"/>
       <c r="AN30" s="4" t="n"/>
-      <c r="AO30" s="4" t="n">
-        <v>0</v>
+      <c r="AO30" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP30" s="4" t="n">
         <v>10503.12</v>
@@ -4849,11 +4793,7 @@
       <c r="AV30" s="4" t="n"/>
       <c r="AW30" s="4" t="n"/>
       <c r="AX30" s="4" t="n"/>
-      <c r="AY30" s="4" t="inlineStr">
-        <is>
-          <t>K1115289.136033118.20251010T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY30" s="4" t="n"/>
       <c r="AZ30" s="4" t="n"/>
       <c r="BA30" s="4" t="n"/>
       <c r="BB30" s="4" t="n"/>
@@ -4914,13 +4854,13 @@
           <t>7th Floor, 33 Cavendish Square, London W1G 0PW, United Kingdom</t>
         </is>
       </c>
-      <c r="Y31" s="4" t="n"/>
+      <c r="Y31" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z31" s="4" t="n"/>
-      <c r="AA31" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA31" s="4" t="n"/>
       <c r="AB31" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -4942,8 +4882,10 @@
       <c r="AL31" s="4" t="n"/>
       <c r="AM31" s="4" t="n"/>
       <c r="AN31" s="4" t="n"/>
-      <c r="AO31" s="4" t="n">
-        <v>0</v>
+      <c r="AO31" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP31" s="4" t="n">
         <v>12109.18</v>
@@ -4960,11 +4902,7 @@
       <c r="AV31" s="4" t="n"/>
       <c r="AW31" s="4" t="n"/>
       <c r="AX31" s="4" t="n"/>
-      <c r="AY31" s="4" t="inlineStr">
-        <is>
-          <t>K1115289.136202406.20251013T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY31" s="4" t="n"/>
       <c r="AZ31" s="4" t="n"/>
       <c r="BA31" s="4" t="n"/>
       <c r="BB31" s="4" t="n"/>
@@ -5025,13 +4963,13 @@
           <t>7th Floor, 33 Cavendish Square, London W1G 0PW, United Kingdom</t>
         </is>
       </c>
-      <c r="Y32" s="4" t="n"/>
+      <c r="Y32" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z32" s="4" t="n"/>
-      <c r="AA32" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA32" s="4" t="n"/>
       <c r="AB32" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -5053,8 +4991,10 @@
       <c r="AL32" s="4" t="n"/>
       <c r="AM32" s="4" t="n"/>
       <c r="AN32" s="4" t="n"/>
-      <c r="AO32" s="4" t="n">
-        <v>0</v>
+      <c r="AO32" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP32" s="4" t="n">
         <v>10573.56</v>
@@ -5071,11 +5011,7 @@
       <c r="AV32" s="4" t="n"/>
       <c r="AW32" s="4" t="n"/>
       <c r="AX32" s="4" t="n"/>
-      <c r="AY32" s="4" t="inlineStr">
-        <is>
-          <t>K1115289.136323385.20251015T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY32" s="4" t="n"/>
       <c r="AZ32" s="4" t="n"/>
       <c r="BA32" s="4" t="n"/>
       <c r="BB32" s="4" t="n"/>
@@ -5136,13 +5072,13 @@
           <t>10 York Road, London SE1 7ND, United Kingdom</t>
         </is>
       </c>
-      <c r="Y33" s="4" t="n"/>
+      <c r="Y33" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z33" s="4" t="n"/>
-      <c r="AA33" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA33" s="4" t="n"/>
       <c r="AB33" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -5164,8 +5100,10 @@
       <c r="AL33" s="4" t="n"/>
       <c r="AM33" s="4" t="n"/>
       <c r="AN33" s="4" t="n"/>
-      <c r="AO33" s="4" t="n">
-        <v>0</v>
+      <c r="AO33" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP33" s="4" t="n">
         <v>9588.360000000001</v>
@@ -5182,11 +5120,7 @@
       <c r="AV33" s="4" t="n"/>
       <c r="AW33" s="4" t="n"/>
       <c r="AX33" s="4" t="n"/>
-      <c r="AY33" s="4" t="inlineStr">
-        <is>
-          <t>K1115289.136470863.20251017T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY33" s="4" t="n"/>
       <c r="AZ33" s="4" t="n"/>
       <c r="BA33" s="4" t="n"/>
       <c r="BB33" s="4" t="n"/>
@@ -5247,13 +5181,13 @@
           <t>10 York Road, London SE1 7ND, United Kingdom</t>
         </is>
       </c>
-      <c r="Y34" s="4" t="n"/>
+      <c r="Y34" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z34" s="4" t="n"/>
-      <c r="AA34" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA34" s="4" t="n"/>
       <c r="AB34" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -5275,8 +5209,10 @@
       <c r="AL34" s="4" t="n"/>
       <c r="AM34" s="4" t="n"/>
       <c r="AN34" s="4" t="n"/>
-      <c r="AO34" s="4" t="n">
-        <v>0</v>
+      <c r="AO34" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP34" s="4" t="n">
         <v>11337.63</v>
@@ -5293,11 +5229,7 @@
       <c r="AV34" s="4" t="n"/>
       <c r="AW34" s="4" t="n"/>
       <c r="AX34" s="4" t="n"/>
-      <c r="AY34" s="4" t="inlineStr">
-        <is>
-          <t>K1115289.136639491.20251020T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY34" s="4" t="n"/>
       <c r="AZ34" s="4" t="n"/>
       <c r="BA34" s="4" t="n"/>
       <c r="BB34" s="4" t="n"/>
@@ -5358,13 +5290,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y35" s="4" t="n"/>
+      <c r="Y35" s="4" t="inlineStr">
+        <is>
+          <t>PLN</t>
+        </is>
+      </c>
       <c r="Z35" s="4" t="n"/>
-      <c r="AA35" s="4" t="inlineStr">
-        <is>
-          <t>PLN</t>
-        </is>
-      </c>
+      <c r="AA35" s="4" t="n"/>
       <c r="AB35" s="4" t="inlineStr">
         <is>
           <t>2nd Floor, 12 Victoria Buildings Haddington Road, Dublin, D04 XN32</t>
@@ -5386,8 +5318,10 @@
       <c r="AL35" s="4" t="n"/>
       <c r="AM35" s="4" t="n"/>
       <c r="AN35" s="4" t="n"/>
-      <c r="AO35" s="4" t="n">
-        <v>0</v>
+      <c r="AO35" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP35" s="4" t="n">
         <v>0</v>
@@ -5404,11 +5338,7 @@
       <c r="AV35" s="4" t="n"/>
       <c r="AW35" s="4" t="n"/>
       <c r="AX35" s="4" t="n"/>
-      <c r="AY35" s="4" t="inlineStr">
-        <is>
-          <t>K6667739.SHEIN135526417.20251002T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY35" s="4" t="n"/>
       <c r="AZ35" s="4" t="n"/>
       <c r="BA35" s="4" t="n"/>
       <c r="BB35" s="4" t="n"/>
@@ -5469,13 +5399,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y36" s="4" t="n"/>
+      <c r="Y36" s="4" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
       <c r="Z36" s="4" t="n"/>
-      <c r="AA36" s="4" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
+      <c r="AA36" s="4" t="n"/>
       <c r="AB36" s="4" t="inlineStr">
         <is>
           <t>2nd Floor, 12 Victoria Buildings Haddington Road, Dublin, D04 XN32</t>
@@ -5497,8 +5427,10 @@
       <c r="AL36" s="4" t="n"/>
       <c r="AM36" s="4" t="n"/>
       <c r="AN36" s="4" t="n"/>
-      <c r="AO36" s="4" t="n">
-        <v>0</v>
+      <c r="AO36" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP36" s="4" t="n">
         <v>0</v>
@@ -5515,11 +5447,7 @@
       <c r="AV36" s="4" t="n"/>
       <c r="AW36" s="4" t="n"/>
       <c r="AX36" s="4" t="n"/>
-      <c r="AY36" s="4" t="inlineStr">
-        <is>
-          <t>K6667739.SHEIN135762026.20251006T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY36" s="4" t="n"/>
       <c r="AZ36" s="4" t="n"/>
       <c r="BA36" s="4" t="n"/>
       <c r="BB36" s="4" t="n"/>
@@ -5580,13 +5508,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y37" s="4" t="n"/>
+      <c r="Y37" s="4" t="inlineStr">
+        <is>
+          <t>NOK</t>
+        </is>
+      </c>
       <c r="Z37" s="4" t="n"/>
-      <c r="AA37" s="4" t="inlineStr">
-        <is>
-          <t>NOK</t>
-        </is>
-      </c>
+      <c r="AA37" s="4" t="n"/>
       <c r="AB37" s="4" t="inlineStr">
         <is>
           <t>2nd Floor, 12 Victoria Buildings Haddington Road, Dublin, D04 XN32</t>
@@ -5608,8 +5536,10 @@
       <c r="AL37" s="4" t="n"/>
       <c r="AM37" s="4" t="n"/>
       <c r="AN37" s="4" t="n"/>
-      <c r="AO37" s="4" t="n">
-        <v>0</v>
+      <c r="AO37" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP37" s="4" t="n">
         <v>0</v>
@@ -5626,11 +5556,7 @@
       <c r="AV37" s="4" t="n"/>
       <c r="AW37" s="4" t="n"/>
       <c r="AX37" s="4" t="n"/>
-      <c r="AY37" s="4" t="inlineStr">
-        <is>
-          <t>K6667739.SHEIN136154303.20251012T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY37" s="4" t="n"/>
       <c r="AZ37" s="4" t="n"/>
       <c r="BA37" s="4" t="n"/>
       <c r="BB37" s="4" t="n"/>
@@ -5691,13 +5617,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y38" s="4" t="n"/>
+      <c r="Y38" s="4" t="inlineStr">
+        <is>
+          <t>HUF</t>
+        </is>
+      </c>
       <c r="Z38" s="4" t="n"/>
-      <c r="AA38" s="4" t="inlineStr">
-        <is>
-          <t>HUF</t>
-        </is>
-      </c>
+      <c r="AA38" s="4" t="n"/>
       <c r="AB38" s="4" t="inlineStr">
         <is>
           <t>2nd Floor, 12 Victoria Buildings Haddington Road, Dublin, D04 XN32</t>
@@ -5719,8 +5645,10 @@
       <c r="AL38" s="4" t="n"/>
       <c r="AM38" s="4" t="n"/>
       <c r="AN38" s="4" t="n"/>
-      <c r="AO38" s="4" t="n">
-        <v>0</v>
+      <c r="AO38" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP38" s="4" t="n">
         <v>0</v>
@@ -5737,11 +5665,7 @@
       <c r="AV38" s="4" t="n"/>
       <c r="AW38" s="4" t="n"/>
       <c r="AX38" s="4" t="n"/>
-      <c r="AY38" s="4" t="inlineStr">
-        <is>
-          <t>K6667739.SHEIN136403529.20251016T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY38" s="4" t="n"/>
       <c r="AZ38" s="4" t="n"/>
       <c r="BA38" s="4" t="n"/>
       <c r="BB38" s="4" t="n"/>
@@ -5802,13 +5726,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y39" s="4" t="n"/>
+      <c r="Y39" s="4" t="inlineStr">
+        <is>
+          <t>HUF</t>
+        </is>
+      </c>
       <c r="Z39" s="4" t="n"/>
-      <c r="AA39" s="4" t="inlineStr">
-        <is>
-          <t>HUF</t>
-        </is>
-      </c>
+      <c r="AA39" s="4" t="n"/>
       <c r="AB39" s="4" t="inlineStr">
         <is>
           <t>2nd Floor, 12 Victoria Buildings Haddington Road, Dublin, D04 XN32</t>
@@ -5830,8 +5754,10 @@
       <c r="AL39" s="4" t="n"/>
       <c r="AM39" s="4" t="n"/>
       <c r="AN39" s="4" t="n"/>
-      <c r="AO39" s="4" t="n">
-        <v>0</v>
+      <c r="AO39" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP39" s="4" t="n">
         <v>0</v>
@@ -5848,11 +5774,7 @@
       <c r="AV39" s="4" t="n"/>
       <c r="AW39" s="4" t="n"/>
       <c r="AX39" s="4" t="n"/>
-      <c r="AY39" s="4" t="inlineStr">
-        <is>
-          <t>K6667739.SHEIN136760575.20251022T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY39" s="4" t="n"/>
       <c r="AZ39" s="4" t="n"/>
       <c r="BA39" s="4" t="n"/>
       <c r="BB39" s="4" t="n"/>
@@ -5913,13 +5835,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y40" s="4" t="n"/>
+      <c r="Y40" s="4" t="inlineStr">
+        <is>
+          <t>DKK</t>
+        </is>
+      </c>
       <c r="Z40" s="4" t="n"/>
-      <c r="AA40" s="4" t="inlineStr">
-        <is>
-          <t>DKK</t>
-        </is>
-      </c>
+      <c r="AA40" s="4" t="n"/>
       <c r="AB40" s="4" t="inlineStr">
         <is>
           <t>2nd Floor, 12 Victoria Buildings Haddington Road, Dublin, D04 XN32</t>
@@ -5941,8 +5863,10 @@
       <c r="AL40" s="4" t="n"/>
       <c r="AM40" s="4" t="n"/>
       <c r="AN40" s="4" t="n"/>
-      <c r="AO40" s="4" t="n">
-        <v>0</v>
+      <c r="AO40" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP40" s="4" t="n">
         <v>0</v>
@@ -5959,11 +5883,7 @@
       <c r="AV40" s="4" t="n"/>
       <c r="AW40" s="4" t="n"/>
       <c r="AX40" s="4" t="n"/>
-      <c r="AY40" s="4" t="inlineStr">
-        <is>
-          <t>K6667739.SHEIN136840111.20251023T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY40" s="4" t="n"/>
       <c r="AZ40" s="4" t="n"/>
       <c r="BA40" s="4" t="n"/>
       <c r="BB40" s="4" t="n"/>
@@ -6024,13 +5944,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y41" s="4" t="n"/>
+      <c r="Y41" s="4" t="inlineStr">
+        <is>
+          <t>SEK</t>
+        </is>
+      </c>
       <c r="Z41" s="4" t="n"/>
-      <c r="AA41" s="4" t="inlineStr">
-        <is>
-          <t>SEK</t>
-        </is>
-      </c>
+      <c r="AA41" s="4" t="n"/>
       <c r="AB41" s="4" t="inlineStr">
         <is>
           <t>2nd Floor, 12 Victoria Buildings Haddington Road, Dublin, D04 XN32</t>
@@ -6052,8 +5972,10 @@
       <c r="AL41" s="4" t="n"/>
       <c r="AM41" s="4" t="n"/>
       <c r="AN41" s="4" t="n"/>
-      <c r="AO41" s="4" t="n">
-        <v>0</v>
+      <c r="AO41" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP41" s="4" t="n">
         <v>0</v>
@@ -6070,11 +5992,7 @@
       <c r="AV41" s="4" t="n"/>
       <c r="AW41" s="4" t="n"/>
       <c r="AX41" s="4" t="n"/>
-      <c r="AY41" s="4" t="inlineStr">
-        <is>
-          <t>K6667739.SHEIN137033972.20251026T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY41" s="4" t="n"/>
       <c r="AZ41" s="4" t="n"/>
       <c r="BA41" s="4" t="n"/>
       <c r="BB41" s="4" t="n"/>
@@ -6135,13 +6053,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y42" s="4" t="n"/>
+      <c r="Y42" s="4" t="inlineStr">
+        <is>
+          <t>RON</t>
+        </is>
+      </c>
       <c r="Z42" s="4" t="n"/>
-      <c r="AA42" s="4" t="inlineStr">
-        <is>
-          <t>RON</t>
-        </is>
-      </c>
+      <c r="AA42" s="4" t="n"/>
       <c r="AB42" s="4" t="inlineStr">
         <is>
           <t>2nd Floor, 12 Victoria Buildings Haddington Road, Dublin, D04 XN32</t>
@@ -6163,8 +6081,10 @@
       <c r="AL42" s="4" t="n"/>
       <c r="AM42" s="4" t="n"/>
       <c r="AN42" s="4" t="n"/>
-      <c r="AO42" s="4" t="n">
-        <v>0</v>
+      <c r="AO42" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP42" s="4" t="n">
         <v>0</v>
@@ -6181,11 +6101,7 @@
       <c r="AV42" s="4" t="n"/>
       <c r="AW42" s="4" t="n"/>
       <c r="AX42" s="4" t="n"/>
-      <c r="AY42" s="4" t="inlineStr">
-        <is>
-          <t>K6667739.SHEIN137294656.20251030T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY42" s="4" t="n"/>
       <c r="AZ42" s="4" t="n"/>
       <c r="BA42" s="4" t="n"/>
       <c r="BB42" s="4" t="n"/>
@@ -6246,13 +6162,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y43" s="4" t="n"/>
+      <c r="Y43" s="4" t="inlineStr">
+        <is>
+          <t>RON</t>
+        </is>
+      </c>
       <c r="Z43" s="4" t="n"/>
-      <c r="AA43" s="4" t="inlineStr">
-        <is>
-          <t>RON</t>
-        </is>
-      </c>
+      <c r="AA43" s="4" t="n"/>
       <c r="AB43" s="4" t="inlineStr">
         <is>
           <t>2nd Floor, 12 Victoria Buildings Haddington Road, Dublin, D04 XN32</t>
@@ -6274,8 +6190,10 @@
       <c r="AL43" s="4" t="n"/>
       <c r="AM43" s="4" t="n"/>
       <c r="AN43" s="4" t="n"/>
-      <c r="AO43" s="4" t="n">
-        <v>0</v>
+      <c r="AO43" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP43" s="4" t="n">
         <v>0</v>
@@ -6292,11 +6210,7 @@
       <c r="AV43" s="4" t="n"/>
       <c r="AW43" s="4" t="n"/>
       <c r="AX43" s="4" t="n"/>
-      <c r="AY43" s="4" t="inlineStr">
-        <is>
-          <t>K6667739.SHEIN137361363.20251031T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY43" s="4" t="n"/>
       <c r="AZ43" s="4" t="n"/>
       <c r="BA43" s="4" t="n"/>
       <c r="BB43" s="4" t="n"/>
@@ -6357,13 +6271,13 @@
           <t>Sveavägen 46, 111 34 Stockholm, Sweden</t>
         </is>
       </c>
-      <c r="Y44" s="4" t="n"/>
+      <c r="Y44" s="4" t="inlineStr">
+        <is>
+          <t>EUR</t>
+        </is>
+      </c>
       <c r="Z44" s="4" t="n"/>
-      <c r="AA44" s="4" t="inlineStr">
-        <is>
-          <t>EUR</t>
-        </is>
-      </c>
+      <c r="AA44" s="4" t="n"/>
       <c r="AB44" s="4" t="inlineStr">
         <is>
           <t>2nd Floor, 12 Victoria Buildings Haddington Road, Dublin, D04 XN32</t>
@@ -6385,8 +6299,10 @@
       <c r="AL44" s="4" t="n"/>
       <c r="AM44" s="4" t="n"/>
       <c r="AN44" s="4" t="n"/>
-      <c r="AO44" s="4" t="n">
-        <v>0</v>
+      <c r="AO44" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP44" s="4" t="n">
         <v>0</v>
@@ -6403,11 +6319,7 @@
       <c r="AV44" s="4" t="n"/>
       <c r="AW44" s="4" t="n"/>
       <c r="AX44" s="4" t="n"/>
-      <c r="AY44" s="4" t="inlineStr">
-        <is>
-          <t>K6667739.SHEIN137361366.20251031T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY44" s="4" t="n"/>
       <c r="AZ44" s="4" t="n"/>
       <c r="BA44" s="4" t="n"/>
       <c r="BB44" s="4" t="n"/>
@@ -6468,13 +6380,13 @@
           <t>7th Floor, 33 Cavendish Square, London W1G 0PW, United Kingdom</t>
         </is>
       </c>
-      <c r="Y45" s="4" t="n"/>
+      <c r="Y45" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z45" s="4" t="n"/>
-      <c r="AA45" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA45" s="4" t="n"/>
       <c r="AB45" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -6496,8 +6408,10 @@
       <c r="AL45" s="4" t="n"/>
       <c r="AM45" s="4" t="n"/>
       <c r="AN45" s="4" t="n"/>
-      <c r="AO45" s="4" t="n">
-        <v>0</v>
+      <c r="AO45" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP45" s="4" t="n">
         <v>2636.36</v>
@@ -6514,11 +6428,7 @@
       <c r="AV45" s="4" t="n"/>
       <c r="AW45" s="4" t="n"/>
       <c r="AX45" s="4" t="n"/>
-      <c r="AY45" s="4" t="inlineStr">
-        <is>
-          <t>K6728496.SHEIN135526381.20251002T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY45" s="4" t="n"/>
       <c r="AZ45" s="4" t="n"/>
       <c r="BA45" s="4" t="n"/>
       <c r="BB45" s="4" t="n"/>
@@ -6579,13 +6489,13 @@
           <t>7th Floor, 33 Cavendish Square, London W1G 0PW, United Kingdom</t>
         </is>
       </c>
-      <c r="Y46" s="4" t="n"/>
+      <c r="Y46" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z46" s="4" t="n"/>
-      <c r="AA46" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA46" s="4" t="n"/>
       <c r="AB46" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -6607,8 +6517,10 @@
       <c r="AL46" s="4" t="n"/>
       <c r="AM46" s="4" t="n"/>
       <c r="AN46" s="4" t="n"/>
-      <c r="AO46" s="4" t="n">
-        <v>0</v>
+      <c r="AO46" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP46" s="4" t="n">
         <v>2082.56</v>
@@ -6625,11 +6537,7 @@
       <c r="AV46" s="4" t="n"/>
       <c r="AW46" s="4" t="n"/>
       <c r="AX46" s="4" t="n"/>
-      <c r="AY46" s="4" t="inlineStr">
-        <is>
-          <t>K6728496.SHEIN135884255.20251008T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY46" s="4" t="n"/>
       <c r="AZ46" s="4" t="n"/>
       <c r="BA46" s="4" t="n"/>
       <c r="BB46" s="4" t="n"/>
@@ -6690,13 +6598,13 @@
           <t>7th Floor, 33 Cavendish Square, London W1G 0PW, United Kingdom</t>
         </is>
       </c>
-      <c r="Y47" s="4" t="n"/>
+      <c r="Y47" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z47" s="4" t="n"/>
-      <c r="AA47" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA47" s="4" t="n"/>
       <c r="AB47" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -6718,8 +6626,10 @@
       <c r="AL47" s="4" t="n"/>
       <c r="AM47" s="4" t="n"/>
       <c r="AN47" s="4" t="n"/>
-      <c r="AO47" s="4" t="n">
-        <v>0</v>
+      <c r="AO47" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP47" s="4" t="n">
         <v>1698.62</v>
@@ -6736,11 +6646,7 @@
       <c r="AV47" s="4" t="n"/>
       <c r="AW47" s="4" t="n"/>
       <c r="AX47" s="4" t="n"/>
-      <c r="AY47" s="4" t="inlineStr">
-        <is>
-          <t>K6728496.SHEIN136154737.20251012T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY47" s="4" t="n"/>
       <c r="AZ47" s="4" t="n"/>
       <c r="BA47" s="4" t="n"/>
       <c r="BB47" s="4" t="n"/>
@@ -6801,13 +6707,13 @@
           <t>7th Floor, 33 Cavendish Square, London W1G 0PW, United Kingdom</t>
         </is>
       </c>
-      <c r="Y48" s="4" t="n"/>
+      <c r="Y48" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z48" s="4" t="n"/>
-      <c r="AA48" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA48" s="4" t="n"/>
       <c r="AB48" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -6829,8 +6735,10 @@
       <c r="AL48" s="4" t="n"/>
       <c r="AM48" s="4" t="n"/>
       <c r="AN48" s="4" t="n"/>
-      <c r="AO48" s="4" t="n">
-        <v>0</v>
+      <c r="AO48" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP48" s="4" t="n">
         <v>1976.17</v>
@@ -6847,11 +6755,7 @@
       <c r="AV48" s="4" t="n"/>
       <c r="AW48" s="4" t="n"/>
       <c r="AX48" s="4" t="n"/>
-      <c r="AY48" s="4" t="inlineStr">
-        <is>
-          <t>K6728496.SHEIN136256285.20251014T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY48" s="4" t="n"/>
       <c r="AZ48" s="4" t="n"/>
       <c r="BA48" s="4" t="n"/>
       <c r="BB48" s="4" t="n"/>
@@ -6912,13 +6816,13 @@
           <t>10 York Road, London SE1 7ND, United Kingdom</t>
         </is>
       </c>
-      <c r="Y49" s="4" t="n"/>
+      <c r="Y49" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z49" s="4" t="n"/>
-      <c r="AA49" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA49" s="4" t="n"/>
       <c r="AB49" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -6940,8 +6844,10 @@
       <c r="AL49" s="4" t="n"/>
       <c r="AM49" s="4" t="n"/>
       <c r="AN49" s="4" t="n"/>
-      <c r="AO49" s="4" t="n">
-        <v>0</v>
+      <c r="AO49" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP49" s="4" t="n">
         <v>1914.64</v>
@@ -6958,11 +6864,7 @@
       <c r="AV49" s="4" t="n"/>
       <c r="AW49" s="4" t="n"/>
       <c r="AX49" s="4" t="n"/>
-      <c r="AY49" s="4" t="inlineStr">
-        <is>
-          <t>K6728496.SHEIN136470472.20251017T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY49" s="4" t="n"/>
       <c r="AZ49" s="4" t="n"/>
       <c r="BA49" s="4" t="n"/>
       <c r="BB49" s="4" t="n"/>
@@ -7023,13 +6925,13 @@
           <t>10 York Road, London SE1 7ND, United Kingdom</t>
         </is>
       </c>
-      <c r="Y50" s="4" t="n"/>
+      <c r="Y50" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z50" s="4" t="n"/>
-      <c r="AA50" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA50" s="4" t="n"/>
       <c r="AB50" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -7051,8 +6953,10 @@
       <c r="AL50" s="4" t="n"/>
       <c r="AM50" s="4" t="n"/>
       <c r="AN50" s="4" t="n"/>
-      <c r="AO50" s="4" t="n">
-        <v>0</v>
+      <c r="AO50" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP50" s="4" t="n">
         <v>1998.82</v>
@@ -7069,11 +6973,7 @@
       <c r="AV50" s="4" t="n"/>
       <c r="AW50" s="4" t="n"/>
       <c r="AX50" s="4" t="n"/>
-      <c r="AY50" s="4" t="inlineStr">
-        <is>
-          <t>K6728496.SHEIN136638445.20251020T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY50" s="4" t="n"/>
       <c r="AZ50" s="4" t="n"/>
       <c r="BA50" s="4" t="n"/>
       <c r="BB50" s="4" t="n"/>
@@ -7134,13 +7034,13 @@
           <t>10 York Road, London SE1 7ND, United Kingdom</t>
         </is>
       </c>
-      <c r="Y51" s="4" t="n"/>
+      <c r="Y51" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z51" s="4" t="n"/>
-      <c r="AA51" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA51" s="4" t="n"/>
       <c r="AB51" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -7162,8 +7062,10 @@
       <c r="AL51" s="4" t="n"/>
       <c r="AM51" s="4" t="n"/>
       <c r="AN51" s="4" t="n"/>
-      <c r="AO51" s="4" t="n">
-        <v>0</v>
+      <c r="AO51" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP51" s="4" t="n">
         <v>1509.09</v>
@@ -7180,11 +7082,7 @@
       <c r="AV51" s="4" t="n"/>
       <c r="AW51" s="4" t="n"/>
       <c r="AX51" s="4" t="n"/>
-      <c r="AY51" s="4" t="inlineStr">
-        <is>
-          <t>K6728496.SHEIN136839742.20251023T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY51" s="4" t="n"/>
       <c r="AZ51" s="4" t="n"/>
       <c r="BA51" s="4" t="n"/>
       <c r="BB51" s="4" t="n"/>
@@ -7245,13 +7143,13 @@
           <t>10 York Road, London SE1 7ND, United Kingdom</t>
         </is>
       </c>
-      <c r="Y52" s="4" t="n"/>
+      <c r="Y52" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z52" s="4" t="n"/>
-      <c r="AA52" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA52" s="4" t="n"/>
       <c r="AB52" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -7273,8 +7171,10 @@
       <c r="AL52" s="4" t="n"/>
       <c r="AM52" s="4" t="n"/>
       <c r="AN52" s="4" t="n"/>
-      <c r="AO52" s="4" t="n">
-        <v>0</v>
+      <c r="AO52" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP52" s="4" t="n">
         <v>1884.78</v>
@@ -7291,11 +7191,7 @@
       <c r="AV52" s="4" t="n"/>
       <c r="AW52" s="4" t="n"/>
       <c r="AX52" s="4" t="n"/>
-      <c r="AY52" s="4" t="inlineStr">
-        <is>
-          <t>K6728496.SHEIN137082951.20251027T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY52" s="4" t="n"/>
       <c r="AZ52" s="4" t="n"/>
       <c r="BA52" s="4" t="n"/>
       <c r="BB52" s="4" t="n"/>
@@ -7356,13 +7252,13 @@
           <t>10 York Road, London SE1 7ND, United Kingdom</t>
         </is>
       </c>
-      <c r="Y53" s="4" t="n"/>
+      <c r="Y53" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z53" s="4" t="n"/>
-      <c r="AA53" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA53" s="4" t="n"/>
       <c r="AB53" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -7384,8 +7280,10 @@
       <c r="AL53" s="4" t="n"/>
       <c r="AM53" s="4" t="n"/>
       <c r="AN53" s="4" t="n"/>
-      <c r="AO53" s="4" t="n">
-        <v>0</v>
+      <c r="AO53" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP53" s="4" t="n">
         <v>1809.09</v>
@@ -7402,11 +7300,7 @@
       <c r="AV53" s="4" t="n"/>
       <c r="AW53" s="4" t="n"/>
       <c r="AX53" s="4" t="n"/>
-      <c r="AY53" s="4" t="inlineStr">
-        <is>
-          <t>K6728496.SHEIN137209349.20251029T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY53" s="4" t="n"/>
       <c r="AZ53" s="4" t="n"/>
       <c r="BA53" s="4" t="n"/>
       <c r="BB53" s="4" t="n"/>
@@ -7467,13 +7361,13 @@
           <t>10 York Road, London SE1 7ND, United Kingdom</t>
         </is>
       </c>
-      <c r="Y54" s="4" t="n"/>
+      <c r="Y54" s="4" t="inlineStr">
+        <is>
+          <t>GBP</t>
+        </is>
+      </c>
       <c r="Z54" s="4" t="n"/>
-      <c r="AA54" s="4" t="inlineStr">
-        <is>
-          <t>GBP</t>
-        </is>
-      </c>
+      <c r="AA54" s="4" t="n"/>
       <c r="AB54" s="4" t="inlineStr">
         <is>
           <t>1 Bartholomew Lane, London, EC2N 2AX, GB</t>
@@ -7495,8 +7389,10 @@
       <c r="AL54" s="4" t="n"/>
       <c r="AM54" s="4" t="n"/>
       <c r="AN54" s="4" t="n"/>
-      <c r="AO54" s="4" t="n">
-        <v>0</v>
+      <c r="AO54" s="4" t="inlineStr">
+        <is>
+          <t>20.00 %</t>
+        </is>
       </c>
       <c r="AP54" s="4" t="n">
         <v>1576.94</v>
@@ -7513,11 +7409,7 @@
       <c r="AV54" s="4" t="n"/>
       <c r="AW54" s="4" t="n"/>
       <c r="AX54" s="4" t="n"/>
-      <c r="AY54" s="4" t="inlineStr">
-        <is>
-          <t>K6728496.SHEIN137361054.20251031T000000+0000.txt</t>
-        </is>
-      </c>
+      <c r="AY54" s="4" t="n"/>
       <c r="AZ54" s="4" t="n"/>
       <c r="BA54" s="4" t="n"/>
       <c r="BB54" s="4" t="n"/>
@@ -7578,13 +7470,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y55" s="4" t="n"/>
+      <c r="Y55" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z55" s="4" t="n"/>
-      <c r="AA55" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA55" s="4" t="n"/>
       <c r="AB55" s="4" t="inlineStr">
         <is>
           <t>777 S. Alameda Street, 2nd Floor, Los Angeles, CA, 90021</t>
@@ -7606,8 +7498,10 @@
       <c r="AL55" s="4" t="n"/>
       <c r="AM55" s="4" t="n"/>
       <c r="AN55" s="4" t="n"/>
-      <c r="AO55" s="4" t="n">
-        <v>0</v>
+      <c r="AO55" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP55" s="4" t="n">
         <v>0</v>
@@ -7624,11 +7518,7 @@
       <c r="AV55" s="4" t="n"/>
       <c r="AW55" s="4" t="n"/>
       <c r="AX55" s="4" t="n"/>
-      <c r="AY55" s="4" t="inlineStr">
-        <is>
-          <t>settlement.128354722.txt</t>
-        </is>
-      </c>
+      <c r="AY55" s="4" t="n"/>
       <c r="AZ55" s="4" t="n"/>
       <c r="BA55" s="4" t="n"/>
       <c r="BB55" s="4" t="n"/>
@@ -7689,13 +7579,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y56" s="4" t="n"/>
+      <c r="Y56" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z56" s="4" t="n"/>
-      <c r="AA56" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA56" s="4" t="n"/>
       <c r="AB56" s="4" t="inlineStr">
         <is>
           <t>345 N. Baldwin Park Boulevard City of Industry, CA 91746, Delaware, 19934</t>
@@ -7717,8 +7607,10 @@
       <c r="AL56" s="4" t="n"/>
       <c r="AM56" s="4" t="n"/>
       <c r="AN56" s="4" t="n"/>
-      <c r="AO56" s="4" t="n">
-        <v>0</v>
+      <c r="AO56" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP56" s="4" t="n">
         <v>0</v>
@@ -7735,11 +7627,7 @@
       <c r="AV56" s="4" t="n"/>
       <c r="AW56" s="4" t="n"/>
       <c r="AX56" s="4" t="n"/>
-      <c r="AY56" s="4" t="inlineStr">
-        <is>
-          <t>settlement.128355257.txt</t>
-        </is>
-      </c>
+      <c r="AY56" s="4" t="n"/>
       <c r="AZ56" s="4" t="n"/>
       <c r="BA56" s="4" t="n"/>
       <c r="BB56" s="4" t="n"/>
@@ -7800,13 +7688,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y57" s="4" t="n"/>
+      <c r="Y57" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z57" s="4" t="n"/>
-      <c r="AA57" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA57" s="4" t="n"/>
       <c r="AB57" s="4" t="inlineStr">
         <is>
           <t>777 S. Alameda Street, 2nd Floor, Los Angeles, CA, 90021</t>
@@ -7828,8 +7716,10 @@
       <c r="AL57" s="4" t="n"/>
       <c r="AM57" s="4" t="n"/>
       <c r="AN57" s="4" t="n"/>
-      <c r="AO57" s="4" t="n">
-        <v>0</v>
+      <c r="AO57" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP57" s="4" t="n">
         <v>0</v>
@@ -7846,11 +7736,7 @@
       <c r="AV57" s="4" t="n"/>
       <c r="AW57" s="4" t="n"/>
       <c r="AX57" s="4" t="n"/>
-      <c r="AY57" s="4" t="inlineStr">
-        <is>
-          <t>settlement.128607863.txt</t>
-        </is>
-      </c>
+      <c r="AY57" s="4" t="n"/>
       <c r="AZ57" s="4" t="n"/>
       <c r="BA57" s="4" t="n"/>
       <c r="BB57" s="4" t="n"/>
@@ -7911,13 +7797,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y58" s="4" t="n"/>
+      <c r="Y58" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z58" s="4" t="n"/>
-      <c r="AA58" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA58" s="4" t="n"/>
       <c r="AB58" s="4" t="inlineStr">
         <is>
           <t>345 N. Baldwin Park Boulevard City of Industry, CA 91746, Delaware, 19934</t>
@@ -7939,8 +7825,10 @@
       <c r="AL58" s="4" t="n"/>
       <c r="AM58" s="4" t="n"/>
       <c r="AN58" s="4" t="n"/>
-      <c r="AO58" s="4" t="n">
-        <v>0</v>
+      <c r="AO58" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP58" s="4" t="n">
         <v>0</v>
@@ -7957,11 +7845,7 @@
       <c r="AV58" s="4" t="n"/>
       <c r="AW58" s="4" t="n"/>
       <c r="AX58" s="4" t="n"/>
-      <c r="AY58" s="4" t="inlineStr">
-        <is>
-          <t>settlement.128608218.txt</t>
-        </is>
-      </c>
+      <c r="AY58" s="4" t="n"/>
       <c r="AZ58" s="4" t="n"/>
       <c r="BA58" s="4" t="n"/>
       <c r="BB58" s="4" t="n"/>
@@ -8022,13 +7906,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y59" s="4" t="n"/>
+      <c r="Y59" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z59" s="4" t="n"/>
-      <c r="AA59" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA59" s="4" t="n"/>
       <c r="AB59" s="4" t="inlineStr">
         <is>
           <t>345 N. Baldwin Park Boulevard City of Industry, CA 91746, Delaware, 19934</t>
@@ -8050,8 +7934,10 @@
       <c r="AL59" s="4" t="n"/>
       <c r="AM59" s="4" t="n"/>
       <c r="AN59" s="4" t="n"/>
-      <c r="AO59" s="4" t="n">
-        <v>0</v>
+      <c r="AO59" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP59" s="4" t="n">
         <v>0</v>
@@ -8068,11 +7954,7 @@
       <c r="AV59" s="4" t="n"/>
       <c r="AW59" s="4" t="n"/>
       <c r="AX59" s="4" t="n"/>
-      <c r="AY59" s="4" t="inlineStr">
-        <is>
-          <t>settlement.128665216.txt</t>
-        </is>
-      </c>
+      <c r="AY59" s="4" t="n"/>
       <c r="AZ59" s="4" t="n"/>
       <c r="BA59" s="4" t="n"/>
       <c r="BB59" s="4" t="n"/>
@@ -8133,13 +8015,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y60" s="4" t="n"/>
+      <c r="Y60" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z60" s="4" t="n"/>
-      <c r="AA60" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA60" s="4" t="n"/>
       <c r="AB60" s="4" t="inlineStr">
         <is>
           <t>777 S. Alameda Street, 2nd Floor, Los Angeles, CA, 90021</t>
@@ -8161,8 +8043,10 @@
       <c r="AL60" s="4" t="n"/>
       <c r="AM60" s="4" t="n"/>
       <c r="AN60" s="4" t="n"/>
-      <c r="AO60" s="4" t="n">
-        <v>0</v>
+      <c r="AO60" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP60" s="4" t="n">
         <v>0</v>
@@ -8179,11 +8063,7 @@
       <c r="AV60" s="4" t="n"/>
       <c r="AW60" s="4" t="n"/>
       <c r="AX60" s="4" t="n"/>
-      <c r="AY60" s="4" t="inlineStr">
-        <is>
-          <t>settlement.128759676.txt</t>
-        </is>
-      </c>
+      <c r="AY60" s="4" t="n"/>
       <c r="AZ60" s="4" t="n"/>
       <c r="BA60" s="4" t="n"/>
       <c r="BB60" s="4" t="n"/>
@@ -8244,13 +8124,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y61" s="4" t="n"/>
+      <c r="Y61" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z61" s="4" t="n"/>
-      <c r="AA61" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA61" s="4" t="n"/>
       <c r="AB61" s="4" t="inlineStr">
         <is>
           <t>345 N. Baldwin Park Boulevard City of Industry, CA 91746, Delaware, 19934</t>
@@ -8272,8 +8152,10 @@
       <c r="AL61" s="4" t="n"/>
       <c r="AM61" s="4" t="n"/>
       <c r="AN61" s="4" t="n"/>
-      <c r="AO61" s="4" t="n">
-        <v>0</v>
+      <c r="AO61" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP61" s="4" t="n">
         <v>0</v>
@@ -8290,11 +8172,7 @@
       <c r="AV61" s="4" t="n"/>
       <c r="AW61" s="4" t="n"/>
       <c r="AX61" s="4" t="n"/>
-      <c r="AY61" s="4" t="inlineStr">
-        <is>
-          <t>settlement.128759996.txt</t>
-        </is>
-      </c>
+      <c r="AY61" s="4" t="n"/>
       <c r="AZ61" s="4" t="n"/>
       <c r="BA61" s="4" t="n"/>
       <c r="BB61" s="4" t="n"/>
@@ -8355,13 +8233,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y62" s="4" t="n"/>
+      <c r="Y62" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z62" s="4" t="n"/>
-      <c r="AA62" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA62" s="4" t="n"/>
       <c r="AB62" s="4" t="inlineStr">
         <is>
           <t>777 S. Alameda Street, 2nd Floor, Los Angeles, CA, 90021</t>
@@ -8383,8 +8261,10 @@
       <c r="AL62" s="4" t="n"/>
       <c r="AM62" s="4" t="n"/>
       <c r="AN62" s="4" t="n"/>
-      <c r="AO62" s="4" t="n">
-        <v>0</v>
+      <c r="AO62" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP62" s="4" t="n">
         <v>0</v>
@@ -8401,11 +8281,7 @@
       <c r="AV62" s="4" t="n"/>
       <c r="AW62" s="4" t="n"/>
       <c r="AX62" s="4" t="n"/>
-      <c r="AY62" s="4" t="inlineStr">
-        <is>
-          <t>settlement.128862985.txt</t>
-        </is>
-      </c>
+      <c r="AY62" s="4" t="n"/>
       <c r="AZ62" s="4" t="n"/>
       <c r="BA62" s="4" t="n"/>
       <c r="BB62" s="4" t="n"/>
@@ -8466,13 +8342,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y63" s="4" t="n"/>
+      <c r="Y63" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z63" s="4" t="n"/>
-      <c r="AA63" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA63" s="4" t="n"/>
       <c r="AB63" s="4" t="inlineStr">
         <is>
           <t>345 N. Baldwin Park Boulevard City of Industry, CA 91746, Delaware, 19934</t>
@@ -8494,8 +8370,10 @@
       <c r="AL63" s="4" t="n"/>
       <c r="AM63" s="4" t="n"/>
       <c r="AN63" s="4" t="n"/>
-      <c r="AO63" s="4" t="n">
-        <v>0</v>
+      <c r="AO63" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP63" s="4" t="n">
         <v>0</v>
@@ -8512,11 +8390,7 @@
       <c r="AV63" s="4" t="n"/>
       <c r="AW63" s="4" t="n"/>
       <c r="AX63" s="4" t="n"/>
-      <c r="AY63" s="4" t="inlineStr">
-        <is>
-          <t>settlement.128922574.txt</t>
-        </is>
-      </c>
+      <c r="AY63" s="4" t="n"/>
       <c r="AZ63" s="4" t="n"/>
       <c r="BA63" s="4" t="n"/>
       <c r="BB63" s="4" t="n"/>
@@ -8577,13 +8451,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y64" s="4" t="n"/>
+      <c r="Y64" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z64" s="4" t="n"/>
-      <c r="AA64" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA64" s="4" t="n"/>
       <c r="AB64" s="4" t="inlineStr">
         <is>
           <t>777 S. Alameda Street, 2nd Floor, Los Angeles, CA, 90021</t>
@@ -8605,8 +8479,10 @@
       <c r="AL64" s="4" t="n"/>
       <c r="AM64" s="4" t="n"/>
       <c r="AN64" s="4" t="n"/>
-      <c r="AO64" s="4" t="n">
-        <v>0</v>
+      <c r="AO64" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP64" s="4" t="n">
         <v>0</v>
@@ -8623,11 +8499,7 @@
       <c r="AV64" s="4" t="n"/>
       <c r="AW64" s="4" t="n"/>
       <c r="AX64" s="4" t="n"/>
-      <c r="AY64" s="4" t="inlineStr">
-        <is>
-          <t>settlement.129059456.txt</t>
-        </is>
-      </c>
+      <c r="AY64" s="4" t="n"/>
       <c r="AZ64" s="4" t="n"/>
       <c r="BA64" s="4" t="n"/>
       <c r="BB64" s="4" t="n"/>
@@ -8688,13 +8560,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y65" s="4" t="n"/>
+      <c r="Y65" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z65" s="4" t="n"/>
-      <c r="AA65" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA65" s="4" t="n"/>
       <c r="AB65" s="4" t="inlineStr">
         <is>
           <t>345 N. Baldwin Park Boulevard City of Industry, CA 91746, Delaware, 19934</t>
@@ -8716,8 +8588,10 @@
       <c r="AL65" s="4" t="n"/>
       <c r="AM65" s="4" t="n"/>
       <c r="AN65" s="4" t="n"/>
-      <c r="AO65" s="4" t="n">
-        <v>0</v>
+      <c r="AO65" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP65" s="4" t="n">
         <v>0</v>
@@ -8734,11 +8608,7 @@
       <c r="AV65" s="4" t="n"/>
       <c r="AW65" s="4" t="n"/>
       <c r="AX65" s="4" t="n"/>
-      <c r="AY65" s="4" t="inlineStr">
-        <is>
-          <t>settlement.129113096.txt</t>
-        </is>
-      </c>
+      <c r="AY65" s="4" t="n"/>
       <c r="AZ65" s="4" t="n"/>
       <c r="BA65" s="4" t="n"/>
       <c r="BB65" s="4" t="n"/>
@@ -8799,13 +8669,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y66" s="4" t="n"/>
+      <c r="Y66" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z66" s="4" t="n"/>
-      <c r="AA66" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA66" s="4" t="n"/>
       <c r="AB66" s="4" t="inlineStr">
         <is>
           <t>777 S. Alameda Street, 2nd Floor, Los Angeles, CA, 90021</t>
@@ -8827,8 +8697,10 @@
       <c r="AL66" s="4" t="n"/>
       <c r="AM66" s="4" t="n"/>
       <c r="AN66" s="4" t="n"/>
-      <c r="AO66" s="4" t="n">
-        <v>0</v>
+      <c r="AO66" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP66" s="4" t="n">
         <v>0</v>
@@ -8845,11 +8717,7 @@
       <c r="AV66" s="4" t="n"/>
       <c r="AW66" s="4" t="n"/>
       <c r="AX66" s="4" t="n"/>
-      <c r="AY66" s="4" t="inlineStr">
-        <is>
-          <t>settlement.129154412.txt</t>
-        </is>
-      </c>
+      <c r="AY66" s="4" t="n"/>
       <c r="AZ66" s="4" t="n"/>
       <c r="BA66" s="4" t="n"/>
       <c r="BB66" s="4" t="n"/>
@@ -8910,13 +8778,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y67" s="4" t="n"/>
+      <c r="Y67" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z67" s="4" t="n"/>
-      <c r="AA67" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA67" s="4" t="n"/>
       <c r="AB67" s="4" t="inlineStr">
         <is>
           <t>345 N. Baldwin Park Boulevard City of Industry, CA 91746, Delaware, 19934</t>
@@ -8938,8 +8806,10 @@
       <c r="AL67" s="4" t="n"/>
       <c r="AM67" s="4" t="n"/>
       <c r="AN67" s="4" t="n"/>
-      <c r="AO67" s="4" t="n">
-        <v>0</v>
+      <c r="AO67" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP67" s="4" t="n">
         <v>0</v>
@@ -8956,11 +8826,7 @@
       <c r="AV67" s="4" t="n"/>
       <c r="AW67" s="4" t="n"/>
       <c r="AX67" s="4" t="n"/>
-      <c r="AY67" s="4" t="inlineStr">
-        <is>
-          <t>settlement.129264424.txt</t>
-        </is>
-      </c>
+      <c r="AY67" s="4" t="n"/>
       <c r="AZ67" s="4" t="n"/>
       <c r="BA67" s="4" t="n"/>
       <c r="BB67" s="4" t="n"/>
@@ -9021,13 +8887,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y68" s="4" t="n"/>
+      <c r="Y68" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z68" s="4" t="n"/>
-      <c r="AA68" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA68" s="4" t="n"/>
       <c r="AB68" s="4" t="inlineStr">
         <is>
           <t>777 S. Alameda Street, 2nd Floor, Los Angeles, CA, 90021</t>
@@ -9049,8 +8915,10 @@
       <c r="AL68" s="4" t="n"/>
       <c r="AM68" s="4" t="n"/>
       <c r="AN68" s="4" t="n"/>
-      <c r="AO68" s="4" t="n">
-        <v>0</v>
+      <c r="AO68" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP68" s="4" t="n">
         <v>0</v>
@@ -9067,11 +8935,7 @@
       <c r="AV68" s="4" t="n"/>
       <c r="AW68" s="4" t="n"/>
       <c r="AX68" s="4" t="n"/>
-      <c r="AY68" s="4" t="inlineStr">
-        <is>
-          <t>settlement.129322025.txt</t>
-        </is>
-      </c>
+      <c r="AY68" s="4" t="n"/>
       <c r="AZ68" s="4" t="n"/>
       <c r="BA68" s="4" t="n"/>
       <c r="BB68" s="4" t="n"/>
@@ -9132,13 +8996,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y69" s="4" t="n"/>
+      <c r="Y69" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z69" s="4" t="n"/>
-      <c r="AA69" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA69" s="4" t="n"/>
       <c r="AB69" s="4" t="inlineStr">
         <is>
           <t>345 N. Baldwin Park Boulevard City of Industry, CA 91746, Delaware, 19934</t>
@@ -9160,8 +9024,10 @@
       <c r="AL69" s="4" t="n"/>
       <c r="AM69" s="4" t="n"/>
       <c r="AN69" s="4" t="n"/>
-      <c r="AO69" s="4" t="n">
-        <v>0</v>
+      <c r="AO69" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP69" s="4" t="n">
         <v>0</v>
@@ -9178,11 +9044,7 @@
       <c r="AV69" s="4" t="n"/>
       <c r="AW69" s="4" t="n"/>
       <c r="AX69" s="4" t="n"/>
-      <c r="AY69" s="4" t="inlineStr">
-        <is>
-          <t>settlement.129455038.txt</t>
-        </is>
-      </c>
+      <c r="AY69" s="4" t="n"/>
       <c r="AZ69" s="4" t="n"/>
       <c r="BA69" s="4" t="n"/>
       <c r="BB69" s="4" t="n"/>
@@ -9243,13 +9105,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y70" s="4" t="n"/>
+      <c r="Y70" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z70" s="4" t="n"/>
-      <c r="AA70" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA70" s="4" t="n"/>
       <c r="AB70" s="4" t="inlineStr">
         <is>
           <t>777 S. Alameda Street, 2nd Floor, Los Angeles, CA, 90021</t>
@@ -9271,8 +9133,10 @@
       <c r="AL70" s="4" t="n"/>
       <c r="AM70" s="4" t="n"/>
       <c r="AN70" s="4" t="n"/>
-      <c r="AO70" s="4" t="n">
-        <v>0</v>
+      <c r="AO70" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP70" s="4" t="n">
         <v>0</v>
@@ -9289,11 +9153,7 @@
       <c r="AV70" s="4" t="n"/>
       <c r="AW70" s="4" t="n"/>
       <c r="AX70" s="4" t="n"/>
-      <c r="AY70" s="4" t="inlineStr">
-        <is>
-          <t>settlement.129543325.txt</t>
-        </is>
-      </c>
+      <c r="AY70" s="4" t="n"/>
       <c r="AZ70" s="4" t="n"/>
       <c r="BA70" s="4" t="n"/>
       <c r="BB70" s="4" t="n"/>
@@ -9354,13 +9214,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y71" s="4" t="n"/>
+      <c r="Y71" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z71" s="4" t="n"/>
-      <c r="AA71" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA71" s="4" t="n"/>
       <c r="AB71" s="4" t="inlineStr">
         <is>
           <t>777 S. Alameda Street, 2nd Floor, Los Angeles, CA, 90021</t>
@@ -9382,8 +9242,10 @@
       <c r="AL71" s="4" t="n"/>
       <c r="AM71" s="4" t="n"/>
       <c r="AN71" s="4" t="n"/>
-      <c r="AO71" s="4" t="n">
-        <v>0</v>
+      <c r="AO71" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP71" s="4" t="n">
         <v>0</v>
@@ -9400,11 +9262,7 @@
       <c r="AV71" s="4" t="n"/>
       <c r="AW71" s="4" t="n"/>
       <c r="AX71" s="4" t="n"/>
-      <c r="AY71" s="4" t="inlineStr">
-        <is>
-          <t>settlement.129650916.txt</t>
-        </is>
-      </c>
+      <c r="AY71" s="4" t="n"/>
       <c r="AZ71" s="4" t="n"/>
       <c r="BA71" s="4" t="n"/>
       <c r="BB71" s="4" t="n"/>
@@ -9465,13 +9323,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y72" s="4" t="n"/>
+      <c r="Y72" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z72" s="4" t="n"/>
-      <c r="AA72" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA72" s="4" t="n"/>
       <c r="AB72" s="4" t="inlineStr">
         <is>
           <t>777 S. Alameda Street, 2nd Floor, Los Angeles, CA, 90021</t>
@@ -9493,8 +9351,10 @@
       <c r="AL72" s="4" t="n"/>
       <c r="AM72" s="4" t="n"/>
       <c r="AN72" s="4" t="n"/>
-      <c r="AO72" s="4" t="n">
-        <v>0</v>
+      <c r="AO72" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP72" s="4" t="n">
         <v>0</v>
@@ -9511,11 +9371,7 @@
       <c r="AV72" s="4" t="n"/>
       <c r="AW72" s="4" t="n"/>
       <c r="AX72" s="4" t="n"/>
-      <c r="AY72" s="4" t="inlineStr">
-        <is>
-          <t>settlement.129708696.txt</t>
-        </is>
-      </c>
+      <c r="AY72" s="4" t="n"/>
       <c r="AZ72" s="4" t="n"/>
       <c r="BA72" s="4" t="n"/>
       <c r="BB72" s="4" t="n"/>
@@ -9576,13 +9432,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y73" s="4" t="n"/>
+      <c r="Y73" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z73" s="4" t="n"/>
-      <c r="AA73" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA73" s="4" t="n"/>
       <c r="AB73" s="4" t="inlineStr">
         <is>
           <t>345 N. Baldwin Park Boulevard City of Industry, CA 91746, Delaware, 19934</t>
@@ -9604,8 +9460,10 @@
       <c r="AL73" s="4" t="n"/>
       <c r="AM73" s="4" t="n"/>
       <c r="AN73" s="4" t="n"/>
-      <c r="AO73" s="4" t="n">
-        <v>0</v>
+      <c r="AO73" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP73" s="4" t="n">
         <v>0</v>
@@ -9622,11 +9480,7 @@
       <c r="AV73" s="4" t="n"/>
       <c r="AW73" s="4" t="n"/>
       <c r="AX73" s="4" t="n"/>
-      <c r="AY73" s="4" t="inlineStr">
-        <is>
-          <t>settlement.129709106.txt</t>
-        </is>
-      </c>
+      <c r="AY73" s="4" t="n"/>
       <c r="AZ73" s="4" t="n"/>
       <c r="BA73" s="4" t="n"/>
       <c r="BB73" s="4" t="n"/>
@@ -9687,13 +9541,13 @@
           <t>800 N High Street, Columbus, OH 43215</t>
         </is>
       </c>
-      <c r="Y74" s="4" t="n"/>
+      <c r="Y74" s="4" t="inlineStr">
+        <is>
+          <t>USD</t>
+        </is>
+      </c>
       <c r="Z74" s="4" t="n"/>
-      <c r="AA74" s="4" t="inlineStr">
-        <is>
-          <t>USD</t>
-        </is>
-      </c>
+      <c r="AA74" s="4" t="n"/>
       <c r="AB74" s="4" t="inlineStr">
         <is>
           <t>345 N. Baldwin Park Boulevard City of Industry, CA 91746, Delaware, 19934</t>
@@ -9715,8 +9569,10 @@
       <c r="AL74" s="4" t="n"/>
       <c r="AM74" s="4" t="n"/>
       <c r="AN74" s="4" t="n"/>
-      <c r="AO74" s="4" t="n">
-        <v>0</v>
+      <c r="AO74" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP74" s="4" t="n">
         <v>0</v>
@@ -9733,11 +9589,7 @@
       <c r="AV74" s="4" t="n"/>
       <c r="AW74" s="4" t="n"/>
       <c r="AX74" s="4" t="n"/>
-      <c r="AY74" s="4" t="inlineStr">
-        <is>
-          <t>settlement.129846305.txt</t>
-        </is>
-      </c>
+      <c r="AY74" s="4" t="n"/>
       <c r="AZ74" s="4" t="n"/>
       <c r="BA74" s="4" t="n"/>
       <c r="BB74" s="4" t="n"/>
@@ -9798,13 +9650,13 @@
           <t>Three Bentall Centre, Suite 2600, 595 Burrard Street, Vancouver, BC, V7X 1L3, Canada</t>
         </is>
       </c>
-      <c r="Y75" s="4" t="n"/>
+      <c r="Y75" s="4" t="inlineStr">
+        <is>
+          <t>CAD</t>
+        </is>
+      </c>
       <c r="Z75" s="4" t="n"/>
-      <c r="AA75" s="4" t="inlineStr">
-        <is>
-          <t>CAD</t>
-        </is>
-      </c>
+      <c r="AA75" s="4" t="n"/>
       <c r="AB75" s="4" t="inlineStr">
         <is>
           <t>10 Caneld Dr, Markham, L3S 3J1, CA</t>
@@ -9826,8 +9678,10 @@
       <c r="AL75" s="4" t="n"/>
       <c r="AM75" s="4" t="n"/>
       <c r="AN75" s="4" t="n"/>
-      <c r="AO75" s="4" t="n">
-        <v>0</v>
+      <c r="AO75" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP75" s="4" t="n">
         <v>0</v>
@@ -9844,11 +9698,7 @@
       <c r="AV75" s="4" t="n"/>
       <c r="AW75" s="4" t="n"/>
       <c r="AX75" s="4" t="n"/>
-      <c r="AY75" s="4" t="inlineStr">
-        <is>
-          <t>settlement.135493701.txt</t>
-        </is>
-      </c>
+      <c r="AY75" s="4" t="n"/>
       <c r="AZ75" s="4" t="n"/>
       <c r="BA75" s="4" t="n"/>
       <c r="BB75" s="4" t="n"/>
@@ -9909,13 +9759,13 @@
           <t>Three Bentall Centre, Suite 2600, 595 Burrard Street, Vancouver, BC, V7X 1L3, Canada</t>
         </is>
       </c>
-      <c r="Y76" s="4" t="n"/>
+      <c r="Y76" s="4" t="inlineStr">
+        <is>
+          <t>CAD</t>
+        </is>
+      </c>
       <c r="Z76" s="4" t="n"/>
-      <c r="AA76" s="4" t="inlineStr">
-        <is>
-          <t>CAD</t>
-        </is>
-      </c>
+      <c r="AA76" s="4" t="n"/>
       <c r="AB76" s="4" t="inlineStr">
         <is>
           <t>10 Caneld Dr, Markham, L3S 3J1, CA</t>
@@ -9937,8 +9787,10 @@
       <c r="AL76" s="4" t="n"/>
       <c r="AM76" s="4" t="n"/>
       <c r="AN76" s="4" t="n"/>
-      <c r="AO76" s="4" t="n">
-        <v>0</v>
+      <c r="AO76" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP76" s="4" t="n">
         <v>0</v>
@@ -9955,11 +9807,7 @@
       <c r="AV76" s="4" t="n"/>
       <c r="AW76" s="4" t="n"/>
       <c r="AX76" s="4" t="n"/>
-      <c r="AY76" s="4" t="inlineStr">
-        <is>
-          <t>settlement.135579529.txt</t>
-        </is>
-      </c>
+      <c r="AY76" s="4" t="n"/>
       <c r="AZ76" s="4" t="n"/>
       <c r="BA76" s="4" t="n"/>
       <c r="BB76" s="4" t="n"/>
@@ -10020,13 +9868,13 @@
           <t>Three Bentall Centre, Suite 2600, 595 Burrard Street, Vancouver, BC, V7X 1L3, Canada</t>
         </is>
       </c>
-      <c r="Y77" s="4" t="n"/>
+      <c r="Y77" s="4" t="inlineStr">
+        <is>
+          <t>CAD</t>
+        </is>
+      </c>
       <c r="Z77" s="4" t="n"/>
-      <c r="AA77" s="4" t="inlineStr">
-        <is>
-          <t>CAD</t>
-        </is>
-      </c>
+      <c r="AA77" s="4" t="n"/>
       <c r="AB77" s="4" t="inlineStr">
         <is>
           <t>10 Caneld Dr, Markham, L3S 3J1, CA</t>
@@ -10048,8 +9896,10 @@
       <c r="AL77" s="4" t="n"/>
       <c r="AM77" s="4" t="n"/>
       <c r="AN77" s="4" t="n"/>
-      <c r="AO77" s="4" t="n">
-        <v>0</v>
+      <c r="AO77" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP77" s="4" t="n">
         <v>0</v>
@@ -10066,11 +9916,7 @@
       <c r="AV77" s="4" t="n"/>
       <c r="AW77" s="4" t="n"/>
       <c r="AX77" s="4" t="n"/>
-      <c r="AY77" s="4" t="inlineStr">
-        <is>
-          <t>settlement.135702252.txt</t>
-        </is>
-      </c>
+      <c r="AY77" s="4" t="n"/>
       <c r="AZ77" s="4" t="n"/>
       <c r="BA77" s="4" t="n"/>
       <c r="BB77" s="4" t="n"/>
@@ -10131,13 +9977,13 @@
           <t>Three Bentall Centre, Suite 2600, 595 Burrard Street, Vancouver, BC, V7X 1L3, Canada</t>
         </is>
       </c>
-      <c r="Y78" s="4" t="n"/>
+      <c r="Y78" s="4" t="inlineStr">
+        <is>
+          <t>CAD</t>
+        </is>
+      </c>
       <c r="Z78" s="4" t="n"/>
-      <c r="AA78" s="4" t="inlineStr">
-        <is>
-          <t>CAD</t>
-        </is>
-      </c>
+      <c r="AA78" s="4" t="n"/>
       <c r="AB78" s="4" t="inlineStr">
         <is>
           <t>10 Caneld Dr, Markham, L3S 3J1, CA</t>
@@ -10159,8 +10005,10 @@
       <c r="AL78" s="4" t="n"/>
       <c r="AM78" s="4" t="n"/>
       <c r="AN78" s="4" t="n"/>
-      <c r="AO78" s="4" t="n">
-        <v>0</v>
+      <c r="AO78" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP78" s="4" t="n">
         <v>0</v>
@@ -10177,11 +10025,7 @@
       <c r="AV78" s="4" t="n"/>
       <c r="AW78" s="4" t="n"/>
       <c r="AX78" s="4" t="n"/>
-      <c r="AY78" s="4" t="inlineStr">
-        <is>
-          <t>settlement.135801582.txt</t>
-        </is>
-      </c>
+      <c r="AY78" s="4" t="n"/>
       <c r="AZ78" s="4" t="n"/>
       <c r="BA78" s="4" t="n"/>
       <c r="BB78" s="4" t="n"/>
@@ -10242,13 +10086,13 @@
           <t>Three Bentall Centre, Suite 2600, 595 Burrard Street, Vancouver, BC, V7X 1L3, Canada</t>
         </is>
       </c>
-      <c r="Y79" s="4" t="n"/>
+      <c r="Y79" s="4" t="inlineStr">
+        <is>
+          <t>CAD</t>
+        </is>
+      </c>
       <c r="Z79" s="4" t="n"/>
-      <c r="AA79" s="4" t="inlineStr">
-        <is>
-          <t>CAD</t>
-        </is>
-      </c>
+      <c r="AA79" s="4" t="n"/>
       <c r="AB79" s="4" t="inlineStr">
         <is>
           <t>10 Caneld Dr, Markham, L3S 3J1, CA</t>
@@ -10270,8 +10114,10 @@
       <c r="AL79" s="4" t="n"/>
       <c r="AM79" s="4" t="n"/>
       <c r="AN79" s="4" t="n"/>
-      <c r="AO79" s="4" t="n">
-        <v>0</v>
+      <c r="AO79" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP79" s="4" t="n">
         <v>0</v>
@@ -10288,11 +10134,7 @@
       <c r="AV79" s="4" t="n"/>
       <c r="AW79" s="4" t="n"/>
       <c r="AX79" s="4" t="n"/>
-      <c r="AY79" s="4" t="inlineStr">
-        <is>
-          <t>settlement.135872340.txt</t>
-        </is>
-      </c>
+      <c r="AY79" s="4" t="n"/>
       <c r="AZ79" s="4" t="n"/>
       <c r="BA79" s="4" t="n"/>
       <c r="BB79" s="4" t="n"/>
@@ -10353,13 +10195,13 @@
           <t>Three Bentall Centre, Suite 2600, 595 Burrard Street, Vancouver, BC, V7X 1L3, Canada</t>
         </is>
       </c>
-      <c r="Y80" s="4" t="n"/>
+      <c r="Y80" s="4" t="inlineStr">
+        <is>
+          <t>CAD</t>
+        </is>
+      </c>
       <c r="Z80" s="4" t="n"/>
-      <c r="AA80" s="4" t="inlineStr">
-        <is>
-          <t>CAD</t>
-        </is>
-      </c>
+      <c r="AA80" s="4" t="n"/>
       <c r="AB80" s="4" t="inlineStr">
         <is>
           <t>10 Caneld Dr, Markham, L3S 3J1, CA</t>
@@ -10381,8 +10223,10 @@
       <c r="AL80" s="4" t="n"/>
       <c r="AM80" s="4" t="n"/>
       <c r="AN80" s="4" t="n"/>
-      <c r="AO80" s="4" t="n">
-        <v>0</v>
+      <c r="AO80" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP80" s="4" t="n">
         <v>0</v>
@@ -10399,11 +10243,7 @@
       <c r="AV80" s="4" t="n"/>
       <c r="AW80" s="4" t="n"/>
       <c r="AX80" s="4" t="n"/>
-      <c r="AY80" s="4" t="inlineStr">
-        <is>
-          <t>settlement.136083809.txt</t>
-        </is>
-      </c>
+      <c r="AY80" s="4" t="n"/>
       <c r="AZ80" s="4" t="n"/>
       <c r="BA80" s="4" t="n"/>
       <c r="BB80" s="4" t="n"/>
@@ -10464,13 +10304,13 @@
           <t>Three Bentall Centre, Suite 2600, 595 Burrard Street, Vancouver, BC, V7X 1L3, Canada</t>
         </is>
       </c>
-      <c r="Y81" s="4" t="n"/>
+      <c r="Y81" s="4" t="inlineStr">
+        <is>
+          <t>CAD</t>
+        </is>
+      </c>
       <c r="Z81" s="4" t="n"/>
-      <c r="AA81" s="4" t="inlineStr">
-        <is>
-          <t>CAD</t>
-        </is>
-      </c>
+      <c r="AA81" s="4" t="n"/>
       <c r="AB81" s="4" t="inlineStr">
         <is>
           <t>10 Caneld Dr, Markham, L3S 3J1, CA</t>
@@ -10492,8 +10332,10 @@
       <c r="AL81" s="4" t="n"/>
       <c r="AM81" s="4" t="n"/>
       <c r="AN81" s="4" t="n"/>
-      <c r="AO81" s="4" t="n">
-        <v>0</v>
+      <c r="AO81" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP81" s="4" t="n">
         <v>0</v>
@@ -10510,11 +10352,7 @@
       <c r="AV81" s="4" t="n"/>
       <c r="AW81" s="4" t="n"/>
       <c r="AX81" s="4" t="n"/>
-      <c r="AY81" s="4" t="inlineStr">
-        <is>
-          <t>settlement.136192944.txt</t>
-        </is>
-      </c>
+      <c r="AY81" s="4" t="n"/>
       <c r="AZ81" s="4" t="n"/>
       <c r="BA81" s="4" t="n"/>
       <c r="BB81" s="4" t="n"/>
@@ -10575,13 +10413,13 @@
           <t>Three Bentall Centre, Suite 2600, 595 Burrard Street, Vancouver, BC, V7X 1L3, Canada</t>
         </is>
       </c>
-      <c r="Y82" s="4" t="n"/>
+      <c r="Y82" s="4" t="inlineStr">
+        <is>
+          <t>CAD</t>
+        </is>
+      </c>
       <c r="Z82" s="4" t="n"/>
-      <c r="AA82" s="4" t="inlineStr">
-        <is>
-          <t>CAD</t>
-        </is>
-      </c>
+      <c r="AA82" s="4" t="n"/>
       <c r="AB82" s="4" t="inlineStr">
         <is>
           <t>10 Caneld Dr, Markham, L3S 3J1, CA</t>
@@ -10603,8 +10441,10 @@
       <c r="AL82" s="4" t="n"/>
       <c r="AM82" s="4" t="n"/>
       <c r="AN82" s="4" t="n"/>
-      <c r="AO82" s="4" t="n">
-        <v>0</v>
+      <c r="AO82" s="4" t="inlineStr">
+        <is>
+          <t>0%</t>
+        </is>
       </c>
       <c r="AP82" s="4" t="n">
         <v>0</v>
@@ -10621,11 +10461,7 @@
       <c r="AV82" s="4" t="n"/>
       <c r="AW82" s="4" t="n"/>
       <c r="AX82" s="4" t="n"/>
-      <c r="AY82" s="4" t="inlineStr">
-        <is>
-          <t>settlement.136581654.txt</t>
-        </is>
-      </c>
+      <c r="AY82" s="4" t="n"/>
       <c r="AZ82" s="4" t="n"/>
       <c r="BA82" s="4" t="n"/>
       <c r="BB82" s="4" t="n"/>

</xml_diff>